<commit_message>
implemented reduced 27 dynamicsÉ
</commit_message>
<xml_diff>
--- a/full dynamics.xlsx
+++ b/full dynamics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/StephaneMagnan/Documents/GitHub/QWOP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D0E9EF-0AA0-D342-B1AA-258C8EF3BA3B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C80E2C4-0B99-1248-8EE7-99C443F611AF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="560" windowWidth="25600" windowHeight="15540" activeTab="2" xr2:uid="{28E72DDC-E907-8543-92E7-F3D54FAF7A29}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3277" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3277" uniqueCount="182">
   <si>
     <t>x</t>
   </si>
@@ -577,6 +577,9 @@
   </si>
   <si>
     <t>-m3*g*gamma3*np.sin(theta3l)-m4*g*(l3)*np.sin(theta3l)-k4*(theta3l+phi4l-theta4l)-c4*(theta3ldot-theta4ldot)+k3*(theta+phi3l-theta3l)+c3*(thetadot-theta3ldot)+fFl*(l3)*np.cos(theta3l)+fNl*(l3)*np.sin(theta3l)</t>
+  </si>
+  <si>
+    <t>-m4*g*gamma4*np.sin(theta4l)+k4*(theta3l+phi4l-theta4l)+c4*(theta3ldot-theta4ldot)+fFl*(l4)*np.cos(theta4l)+fNl*(l4)*np.sin(theta4l)</t>
   </si>
 </sst>
 </file>
@@ -13281,10 +13284,10 @@
   <dimension ref="A1:BI31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="BH4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="BH21" sqref="BH21"/>
+      <selection pane="bottomRight" activeCell="BE30" sqref="C4:BE30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17079,7 +17082,7 @@
         <v>14</v>
       </c>
       <c r="BH22" s="12" t="s">
-        <v>156</v>
+        <v>181</v>
       </c>
       <c r="BI22" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
finalized symbolic solver for 11 equation system for reduced solution time
</commit_message>
<xml_diff>
--- a/full dynamics.xlsx
+++ b/full dynamics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/StephaneMagnan/Documents/GitHub/QWOP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7258E2-5AD6-BF4D-B028-0203DAE12E6D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86F7D37-93A9-3E48-A2CA-F001D78802D6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="560" windowWidth="25600" windowHeight="15540" activeTab="3" xr2:uid="{28E72DDC-E907-8543-92E7-F3D54FAF7A29}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="3" xr2:uid="{28E72DDC-E907-8543-92E7-F3D54FAF7A29}"/>
   </bookViews>
   <sheets>
     <sheet name="31 state" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -623,7 +624,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -765,15 +766,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -783,8 +777,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1108,7 +1109,7 @@
       <selection pane="bottomRight" activeCell="AZ30" sqref="AZ30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
@@ -1181,167 +1182,167 @@
     <col min="69" max="69" width="2.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:69">
       <c r="C1" s="6"/>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="20" t="s">
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="20" t="s">
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="W1" s="18"/>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="18"/>
-      <c r="AB1" s="18"/>
-      <c r="AC1" s="18"/>
-      <c r="AD1" s="18"/>
-      <c r="AE1" s="18"/>
-      <c r="AF1" s="18"/>
-      <c r="AG1" s="18"/>
-      <c r="AH1" s="18"/>
-      <c r="AI1" s="18"/>
-      <c r="AJ1" s="18"/>
-      <c r="AK1" s="19"/>
-      <c r="AL1" s="20" t="s">
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="24"/>
+      <c r="AA1" s="24"/>
+      <c r="AB1" s="24"/>
+      <c r="AC1" s="24"/>
+      <c r="AD1" s="24"/>
+      <c r="AE1" s="24"/>
+      <c r="AF1" s="24"/>
+      <c r="AG1" s="24"/>
+      <c r="AH1" s="24"/>
+      <c r="AI1" s="24"/>
+      <c r="AJ1" s="24"/>
+      <c r="AK1" s="25"/>
+      <c r="AL1" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="AM1" s="18"/>
-      <c r="AN1" s="18"/>
-      <c r="AO1" s="18"/>
-      <c r="AP1" s="18"/>
-      <c r="AQ1" s="18"/>
-      <c r="AR1" s="18"/>
-      <c r="AS1" s="18"/>
-      <c r="AT1" s="18"/>
-      <c r="AU1" s="18"/>
-      <c r="AV1" s="18"/>
-      <c r="AW1" s="19"/>
-      <c r="AX1" s="20" t="s">
+      <c r="AM1" s="24"/>
+      <c r="AN1" s="24"/>
+      <c r="AO1" s="24"/>
+      <c r="AP1" s="24"/>
+      <c r="AQ1" s="24"/>
+      <c r="AR1" s="24"/>
+      <c r="AS1" s="24"/>
+      <c r="AT1" s="24"/>
+      <c r="AU1" s="24"/>
+      <c r="AV1" s="24"/>
+      <c r="AW1" s="25"/>
+      <c r="AX1" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="AY1" s="18"/>
-      <c r="AZ1" s="18"/>
-      <c r="BA1" s="18"/>
-      <c r="BB1" s="18"/>
-      <c r="BC1" s="18"/>
-      <c r="BD1" s="18"/>
-      <c r="BE1" s="18"/>
-      <c r="BF1" s="18"/>
-      <c r="BG1" s="18"/>
-      <c r="BH1" s="18"/>
-      <c r="BI1" s="18"/>
-      <c r="BJ1" s="18"/>
-      <c r="BK1" s="18"/>
-      <c r="BL1" s="18"/>
-      <c r="BM1" s="19"/>
+      <c r="AY1" s="24"/>
+      <c r="AZ1" s="24"/>
+      <c r="BA1" s="24"/>
+      <c r="BB1" s="24"/>
+      <c r="BC1" s="24"/>
+      <c r="BD1" s="24"/>
+      <c r="BE1" s="24"/>
+      <c r="BF1" s="24"/>
+      <c r="BG1" s="24"/>
+      <c r="BH1" s="24"/>
+      <c r="BI1" s="24"/>
+      <c r="BJ1" s="24"/>
+      <c r="BK1" s="24"/>
+      <c r="BL1" s="24"/>
+      <c r="BM1" s="25"/>
     </row>
-    <row r="2" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:69">
       <c r="C2" s="1"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="21" t="s">
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22" t="s">
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="22"/>
-      <c r="T2" s="22"/>
-      <c r="U2" s="23"/>
-      <c r="V2" s="21" t="s">
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="21"/>
+      <c r="T2" s="21"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="W2" s="22"/>
-      <c r="X2" s="22"/>
-      <c r="Y2" s="22"/>
-      <c r="Z2" s="22"/>
-      <c r="AA2" s="22"/>
-      <c r="AB2" s="22" t="s">
+      <c r="W2" s="21"/>
+      <c r="X2" s="21"/>
+      <c r="Y2" s="21"/>
+      <c r="Z2" s="21"/>
+      <c r="AA2" s="21"/>
+      <c r="AB2" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="AC2" s="22"/>
-      <c r="AD2" s="22"/>
-      <c r="AE2" s="22"/>
-      <c r="AF2" s="22"/>
-      <c r="AG2" s="22"/>
-      <c r="AH2" s="22" t="s">
+      <c r="AC2" s="21"/>
+      <c r="AD2" s="21"/>
+      <c r="AE2" s="21"/>
+      <c r="AF2" s="21"/>
+      <c r="AG2" s="21"/>
+      <c r="AH2" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="AI2" s="22"/>
-      <c r="AJ2" s="22"/>
-      <c r="AK2" s="23"/>
-      <c r="AL2" s="21" t="s">
+      <c r="AI2" s="21"/>
+      <c r="AJ2" s="21"/>
+      <c r="AK2" s="22"/>
+      <c r="AL2" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="AM2" s="22"/>
-      <c r="AN2" s="22"/>
-      <c r="AO2" s="22"/>
-      <c r="AP2" s="22"/>
-      <c r="AQ2" s="22"/>
-      <c r="AR2" s="22" t="s">
+      <c r="AM2" s="21"/>
+      <c r="AN2" s="21"/>
+      <c r="AO2" s="21"/>
+      <c r="AP2" s="21"/>
+      <c r="AQ2" s="21"/>
+      <c r="AR2" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="AS2" s="22"/>
-      <c r="AT2" s="22"/>
-      <c r="AU2" s="22"/>
-      <c r="AV2" s="22"/>
-      <c r="AW2" s="23"/>
-      <c r="AX2" s="21" t="s">
+      <c r="AS2" s="21"/>
+      <c r="AT2" s="21"/>
+      <c r="AU2" s="21"/>
+      <c r="AV2" s="21"/>
+      <c r="AW2" s="22"/>
+      <c r="AX2" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="AY2" s="22"/>
-      <c r="AZ2" s="22"/>
-      <c r="BA2" s="22"/>
-      <c r="BB2" s="22"/>
-      <c r="BC2" s="22"/>
-      <c r="BD2" s="22" t="s">
+      <c r="AY2" s="21"/>
+      <c r="AZ2" s="21"/>
+      <c r="BA2" s="21"/>
+      <c r="BB2" s="21"/>
+      <c r="BC2" s="21"/>
+      <c r="BD2" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="BE2" s="22"/>
-      <c r="BF2" s="22"/>
-      <c r="BG2" s="22"/>
-      <c r="BH2" s="22"/>
-      <c r="BI2" s="22"/>
-      <c r="BJ2" s="22" t="s">
+      <c r="BE2" s="21"/>
+      <c r="BF2" s="21"/>
+      <c r="BG2" s="21"/>
+      <c r="BH2" s="21"/>
+      <c r="BI2" s="21"/>
+      <c r="BJ2" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="BK2" s="22"/>
-      <c r="BL2" s="22"/>
-      <c r="BM2" s="23"/>
+      <c r="BK2" s="21"/>
+      <c r="BL2" s="21"/>
+      <c r="BM2" s="22"/>
     </row>
-    <row r="3" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:69">
       <c r="B3" t="s">
         <v>26</v>
       </c>
@@ -1474,7 +1475,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:69">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -1680,7 +1681,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:69">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -1887,7 +1888,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:69">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -2094,7 +2095,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:69">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -2301,7 +2302,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:69">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -2508,7 +2509,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:69">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -2715,7 +2716,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:69">
       <c r="A10" t="s">
         <v>60</v>
       </c>
@@ -2922,7 +2923,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:69">
       <c r="A11" t="s">
         <v>104</v>
       </c>
@@ -3129,7 +3130,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:69">
       <c r="A12" t="s">
         <v>105</v>
       </c>
@@ -3336,7 +3337,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:69">
       <c r="A13" t="s">
         <v>106</v>
       </c>
@@ -3543,7 +3544,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:69">
       <c r="A14" t="s">
         <v>107</v>
       </c>
@@ -3750,7 +3751,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:69">
       <c r="A15" t="s">
         <v>108</v>
       </c>
@@ -3957,7 +3958,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:69">
       <c r="A16" t="s">
         <v>109</v>
       </c>
@@ -4164,7 +4165,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:69">
       <c r="A17" t="s">
         <v>110</v>
       </c>
@@ -4371,7 +4372,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:69">
       <c r="A18" t="s">
         <v>111</v>
       </c>
@@ -4578,7 +4579,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:69">
       <c r="A19" t="s">
         <v>112</v>
       </c>
@@ -4785,7 +4786,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:69">
       <c r="A20" t="s">
         <v>113</v>
       </c>
@@ -4992,7 +4993,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:69">
       <c r="A21" t="s">
         <v>114</v>
       </c>
@@ -5199,7 +5200,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:69">
       <c r="A22" t="s">
         <v>115</v>
       </c>
@@ -5406,7 +5407,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:69">
       <c r="A23" t="s">
         <v>116</v>
       </c>
@@ -5613,7 +5614,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:69">
       <c r="A24" t="s">
         <v>117</v>
       </c>
@@ -5820,7 +5821,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:69">
       <c r="A25" t="s">
         <v>118</v>
       </c>
@@ -6027,7 +6028,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:69">
       <c r="A26" t="s">
         <v>119</v>
       </c>
@@ -6234,7 +6235,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:69">
       <c r="A27" t="s">
         <v>120</v>
       </c>
@@ -6441,7 +6442,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:69">
       <c r="A28" t="s">
         <v>121</v>
       </c>
@@ -6648,7 +6649,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:69">
       <c r="A29" t="s">
         <v>122</v>
       </c>
@@ -6855,7 +6856,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:69">
       <c r="A30" t="s">
         <v>123</v>
       </c>
@@ -7062,7 +7063,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:69">
       <c r="A31" t="s">
         <v>124</v>
       </c>
@@ -7269,7 +7270,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:69">
       <c r="A32" t="s">
         <v>125</v>
       </c>
@@ -7476,7 +7477,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:69">
       <c r="A33" t="s">
         <v>126</v>
       </c>
@@ -7683,7 +7684,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:69">
       <c r="A34" t="s">
         <v>127</v>
       </c>
@@ -7890,7 +7891,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:69">
       <c r="D35" s="11"/>
       <c r="E35" s="11"/>
       <c r="F35" s="11"/>
@@ -7955,6 +7956,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="J1:U1"/>
+    <mergeCell ref="J2:O2"/>
+    <mergeCell ref="P2:U2"/>
+    <mergeCell ref="D2:I2"/>
     <mergeCell ref="AL2:AQ2"/>
     <mergeCell ref="AR2:AW2"/>
     <mergeCell ref="AX2:BC2"/>
@@ -7966,11 +7972,6 @@
     <mergeCell ref="V2:AA2"/>
     <mergeCell ref="AB2:AG2"/>
     <mergeCell ref="AL1:AW1"/>
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="J1:U1"/>
-    <mergeCell ref="J2:O2"/>
-    <mergeCell ref="P2:U2"/>
-    <mergeCell ref="D2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7987,7 +7988,7 @@
       <selection pane="bottomRight" activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
@@ -8052,147 +8053,147 @@
     <col min="61" max="61" width="2.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:61">
       <c r="C1" s="6"/>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="20" t="s">
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="20" t="s">
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="W1" s="18"/>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="18"/>
-      <c r="AB1" s="18"/>
-      <c r="AC1" s="18"/>
-      <c r="AD1" s="18"/>
-      <c r="AE1" s="18"/>
-      <c r="AF1" s="18"/>
-      <c r="AG1" s="19"/>
-      <c r="AH1" s="20" t="s">
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="24"/>
+      <c r="AA1" s="24"/>
+      <c r="AB1" s="24"/>
+      <c r="AC1" s="24"/>
+      <c r="AD1" s="24"/>
+      <c r="AE1" s="24"/>
+      <c r="AF1" s="24"/>
+      <c r="AG1" s="25"/>
+      <c r="AH1" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="AI1" s="18"/>
-      <c r="AJ1" s="18"/>
-      <c r="AK1" s="18"/>
-      <c r="AL1" s="18"/>
-      <c r="AM1" s="18"/>
-      <c r="AN1" s="18"/>
-      <c r="AO1" s="18"/>
-      <c r="AP1" s="18"/>
-      <c r="AQ1" s="18"/>
-      <c r="AR1" s="18"/>
-      <c r="AS1" s="19"/>
-      <c r="AT1" s="20" t="s">
+      <c r="AI1" s="24"/>
+      <c r="AJ1" s="24"/>
+      <c r="AK1" s="24"/>
+      <c r="AL1" s="24"/>
+      <c r="AM1" s="24"/>
+      <c r="AN1" s="24"/>
+      <c r="AO1" s="24"/>
+      <c r="AP1" s="24"/>
+      <c r="AQ1" s="24"/>
+      <c r="AR1" s="24"/>
+      <c r="AS1" s="25"/>
+      <c r="AT1" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="AU1" s="18"/>
-      <c r="AV1" s="18"/>
-      <c r="AW1" s="18"/>
-      <c r="AX1" s="18"/>
-      <c r="AY1" s="18"/>
-      <c r="AZ1" s="18"/>
-      <c r="BA1" s="18"/>
-      <c r="BB1" s="18"/>
-      <c r="BC1" s="18"/>
-      <c r="BD1" s="18"/>
-      <c r="BE1" s="19"/>
+      <c r="AU1" s="24"/>
+      <c r="AV1" s="24"/>
+      <c r="AW1" s="24"/>
+      <c r="AX1" s="24"/>
+      <c r="AY1" s="24"/>
+      <c r="AZ1" s="24"/>
+      <c r="BA1" s="24"/>
+      <c r="BB1" s="24"/>
+      <c r="BC1" s="24"/>
+      <c r="BD1" s="24"/>
+      <c r="BE1" s="25"/>
     </row>
-    <row r="2" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:61">
       <c r="C2" s="1"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="21" t="s">
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22" t="s">
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="22"/>
-      <c r="T2" s="22"/>
-      <c r="U2" s="23"/>
-      <c r="V2" s="21" t="s">
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="21"/>
+      <c r="T2" s="21"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="W2" s="22"/>
-      <c r="X2" s="22"/>
-      <c r="Y2" s="22"/>
-      <c r="Z2" s="22"/>
-      <c r="AA2" s="22"/>
-      <c r="AB2" s="22" t="s">
+      <c r="W2" s="21"/>
+      <c r="X2" s="21"/>
+      <c r="Y2" s="21"/>
+      <c r="Z2" s="21"/>
+      <c r="AA2" s="21"/>
+      <c r="AB2" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="AC2" s="22"/>
-      <c r="AD2" s="22"/>
-      <c r="AE2" s="22"/>
-      <c r="AF2" s="22"/>
+      <c r="AC2" s="21"/>
+      <c r="AD2" s="21"/>
+      <c r="AE2" s="21"/>
+      <c r="AF2" s="21"/>
       <c r="AG2" s="17"/>
-      <c r="AH2" s="21" t="s">
+      <c r="AH2" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="AI2" s="22"/>
-      <c r="AJ2" s="22"/>
-      <c r="AK2" s="22"/>
-      <c r="AL2" s="22"/>
-      <c r="AM2" s="22"/>
-      <c r="AN2" s="22" t="s">
+      <c r="AI2" s="21"/>
+      <c r="AJ2" s="21"/>
+      <c r="AK2" s="21"/>
+      <c r="AL2" s="21"/>
+      <c r="AM2" s="21"/>
+      <c r="AN2" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="AO2" s="22"/>
-      <c r="AP2" s="22"/>
-      <c r="AQ2" s="22"/>
-      <c r="AR2" s="22"/>
-      <c r="AS2" s="23"/>
-      <c r="AT2" s="21" t="s">
+      <c r="AO2" s="21"/>
+      <c r="AP2" s="21"/>
+      <c r="AQ2" s="21"/>
+      <c r="AR2" s="21"/>
+      <c r="AS2" s="22"/>
+      <c r="AT2" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="AU2" s="22"/>
-      <c r="AV2" s="22"/>
-      <c r="AW2" s="22"/>
-      <c r="AX2" s="22"/>
-      <c r="AY2" s="22"/>
-      <c r="AZ2" s="22" t="s">
+      <c r="AU2" s="21"/>
+      <c r="AV2" s="21"/>
+      <c r="AW2" s="21"/>
+      <c r="AX2" s="21"/>
+      <c r="AY2" s="21"/>
+      <c r="AZ2" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="BA2" s="22"/>
-      <c r="BB2" s="22"/>
-      <c r="BC2" s="22"/>
-      <c r="BD2" s="22"/>
+      <c r="BA2" s="21"/>
+      <c r="BB2" s="21"/>
+      <c r="BC2" s="21"/>
+      <c r="BD2" s="21"/>
       <c r="BE2" s="17"/>
     </row>
-    <row r="3" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:61">
       <c r="B3" t="s">
         <v>26</v>
       </c>
@@ -8309,7 +8310,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:61">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -8491,7 +8492,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:61">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -8674,7 +8675,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:61">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -8857,7 +8858,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:61">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -9040,7 +9041,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:61">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -9223,7 +9224,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:61">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -9406,7 +9407,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:61">
       <c r="A10" t="s">
         <v>60</v>
       </c>
@@ -9589,7 +9590,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:61">
       <c r="A11" t="s">
         <v>104</v>
       </c>
@@ -9772,7 +9773,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:61">
       <c r="A12" t="s">
         <v>105</v>
       </c>
@@ -9955,7 +9956,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:61">
       <c r="A13" t="s">
         <v>106</v>
       </c>
@@ -10138,7 +10139,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:61">
       <c r="A14" t="s">
         <v>107</v>
       </c>
@@ -10321,7 +10322,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:61">
       <c r="A15" t="s">
         <v>108</v>
       </c>
@@ -10504,7 +10505,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:61">
       <c r="A16" t="s">
         <v>109</v>
       </c>
@@ -10687,7 +10688,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:61">
       <c r="A17" t="s">
         <v>110</v>
       </c>
@@ -10870,7 +10871,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:61">
       <c r="A18" t="s">
         <v>111</v>
       </c>
@@ -11053,7 +11054,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:61">
       <c r="A19" t="s">
         <v>114</v>
       </c>
@@ -11236,7 +11237,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:61">
       <c r="A20" t="s">
         <v>115</v>
       </c>
@@ -11419,7 +11420,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:61">
       <c r="A21" t="s">
         <v>116</v>
       </c>
@@ -11602,7 +11603,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:61">
       <c r="A22" t="s">
         <v>117</v>
       </c>
@@ -11785,7 +11786,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:61">
       <c r="A23" t="s">
         <v>118</v>
       </c>
@@ -11968,7 +11969,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:61">
       <c r="A24" t="s">
         <v>119</v>
       </c>
@@ -12151,7 +12152,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:61">
       <c r="A25" t="s">
         <v>120</v>
       </c>
@@ -12334,7 +12335,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:61">
       <c r="A26" t="s">
         <v>121</v>
       </c>
@@ -12517,7 +12518,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:61">
       <c r="A27" t="s">
         <v>122</v>
       </c>
@@ -12700,7 +12701,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:61">
       <c r="A28" t="s">
         <v>123</v>
       </c>
@@ -12883,7 +12884,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:61">
       <c r="A29" t="s">
         <v>124</v>
       </c>
@@ -13066,7 +13067,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:61">
       <c r="A30" t="s">
         <v>125</v>
       </c>
@@ -13249,7 +13250,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:61">
       <c r="D31" s="11"/>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
@@ -13336,7 +13337,7 @@
       <selection pane="bottomRight" activeCell="BE30" sqref="C4:BE30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
@@ -13401,147 +13402,147 @@
     <col min="61" max="61" width="2.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:61">
       <c r="C1" s="6"/>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="20" t="s">
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="20" t="s">
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="W1" s="18"/>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="18"/>
-      <c r="AB1" s="18"/>
-      <c r="AC1" s="18"/>
-      <c r="AD1" s="18"/>
-      <c r="AE1" s="18"/>
-      <c r="AF1" s="18"/>
-      <c r="AG1" s="19"/>
-      <c r="AH1" s="20" t="s">
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="24"/>
+      <c r="AA1" s="24"/>
+      <c r="AB1" s="24"/>
+      <c r="AC1" s="24"/>
+      <c r="AD1" s="24"/>
+      <c r="AE1" s="24"/>
+      <c r="AF1" s="24"/>
+      <c r="AG1" s="25"/>
+      <c r="AH1" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="AI1" s="18"/>
-      <c r="AJ1" s="18"/>
-      <c r="AK1" s="18"/>
-      <c r="AL1" s="18"/>
-      <c r="AM1" s="18"/>
-      <c r="AN1" s="18"/>
-      <c r="AO1" s="18"/>
-      <c r="AP1" s="18"/>
-      <c r="AQ1" s="18"/>
-      <c r="AR1" s="18"/>
-      <c r="AS1" s="19"/>
-      <c r="AT1" s="20" t="s">
+      <c r="AI1" s="24"/>
+      <c r="AJ1" s="24"/>
+      <c r="AK1" s="24"/>
+      <c r="AL1" s="24"/>
+      <c r="AM1" s="24"/>
+      <c r="AN1" s="24"/>
+      <c r="AO1" s="24"/>
+      <c r="AP1" s="24"/>
+      <c r="AQ1" s="24"/>
+      <c r="AR1" s="24"/>
+      <c r="AS1" s="25"/>
+      <c r="AT1" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="AU1" s="18"/>
-      <c r="AV1" s="18"/>
-      <c r="AW1" s="18"/>
-      <c r="AX1" s="18"/>
-      <c r="AY1" s="18"/>
-      <c r="AZ1" s="18"/>
-      <c r="BA1" s="18"/>
-      <c r="BB1" s="18"/>
-      <c r="BC1" s="18"/>
-      <c r="BD1" s="18"/>
-      <c r="BE1" s="19"/>
+      <c r="AU1" s="24"/>
+      <c r="AV1" s="24"/>
+      <c r="AW1" s="24"/>
+      <c r="AX1" s="24"/>
+      <c r="AY1" s="24"/>
+      <c r="AZ1" s="24"/>
+      <c r="BA1" s="24"/>
+      <c r="BB1" s="24"/>
+      <c r="BC1" s="24"/>
+      <c r="BD1" s="24"/>
+      <c r="BE1" s="25"/>
     </row>
-    <row r="2" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:61">
       <c r="C2" s="1"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="21" t="s">
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22" t="s">
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="22"/>
-      <c r="T2" s="22"/>
-      <c r="U2" s="23"/>
-      <c r="V2" s="21" t="s">
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="21"/>
+      <c r="T2" s="21"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="W2" s="22"/>
-      <c r="X2" s="22"/>
-      <c r="Y2" s="22"/>
-      <c r="Z2" s="22"/>
-      <c r="AA2" s="22"/>
-      <c r="AB2" s="22" t="s">
+      <c r="W2" s="21"/>
+      <c r="X2" s="21"/>
+      <c r="Y2" s="21"/>
+      <c r="Z2" s="21"/>
+      <c r="AA2" s="21"/>
+      <c r="AB2" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="AC2" s="22"/>
-      <c r="AD2" s="22"/>
-      <c r="AE2" s="22"/>
-      <c r="AF2" s="22"/>
+      <c r="AC2" s="21"/>
+      <c r="AD2" s="21"/>
+      <c r="AE2" s="21"/>
+      <c r="AF2" s="21"/>
       <c r="AG2" s="17"/>
-      <c r="AH2" s="21" t="s">
+      <c r="AH2" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="AI2" s="22"/>
-      <c r="AJ2" s="22"/>
-      <c r="AK2" s="22"/>
-      <c r="AL2" s="22"/>
-      <c r="AM2" s="22"/>
-      <c r="AN2" s="22" t="s">
+      <c r="AI2" s="21"/>
+      <c r="AJ2" s="21"/>
+      <c r="AK2" s="21"/>
+      <c r="AL2" s="21"/>
+      <c r="AM2" s="21"/>
+      <c r="AN2" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="AO2" s="22"/>
-      <c r="AP2" s="22"/>
-      <c r="AQ2" s="22"/>
-      <c r="AR2" s="22"/>
-      <c r="AS2" s="23"/>
-      <c r="AT2" s="21" t="s">
+      <c r="AO2" s="21"/>
+      <c r="AP2" s="21"/>
+      <c r="AQ2" s="21"/>
+      <c r="AR2" s="21"/>
+      <c r="AS2" s="22"/>
+      <c r="AT2" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="AU2" s="22"/>
-      <c r="AV2" s="22"/>
-      <c r="AW2" s="22"/>
-      <c r="AX2" s="22"/>
-      <c r="AY2" s="22"/>
-      <c r="AZ2" s="22" t="s">
+      <c r="AU2" s="21"/>
+      <c r="AV2" s="21"/>
+      <c r="AW2" s="21"/>
+      <c r="AX2" s="21"/>
+      <c r="AY2" s="21"/>
+      <c r="AZ2" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="BA2" s="22"/>
-      <c r="BB2" s="22"/>
-      <c r="BC2" s="22"/>
-      <c r="BD2" s="22"/>
+      <c r="BA2" s="21"/>
+      <c r="BB2" s="21"/>
+      <c r="BC2" s="21"/>
+      <c r="BD2" s="21"/>
       <c r="BE2" s="17"/>
     </row>
-    <row r="3" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:61">
       <c r="B3" t="s">
         <v>26</v>
       </c>
@@ -13658,7 +13659,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:61">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -13840,7 +13841,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:61">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -14023,7 +14024,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:61">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -14206,7 +14207,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:61">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -14389,7 +14390,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:61">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -14572,7 +14573,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:61">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -14755,7 +14756,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:61">
       <c r="A10" t="s">
         <v>60</v>
       </c>
@@ -14938,7 +14939,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:61">
       <c r="A11" t="s">
         <v>104</v>
       </c>
@@ -15121,7 +15122,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:61">
       <c r="A12" t="s">
         <v>105</v>
       </c>
@@ -15304,7 +15305,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:61">
       <c r="A13" t="s">
         <v>106</v>
       </c>
@@ -15487,7 +15488,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:61">
       <c r="A14" t="s">
         <v>107</v>
       </c>
@@ -15670,7 +15671,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:61">
       <c r="A15" t="s">
         <v>108</v>
       </c>
@@ -15853,7 +15854,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:61">
       <c r="A16" t="s">
         <v>109</v>
       </c>
@@ -16036,7 +16037,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:61">
       <c r="A17" t="s">
         <v>110</v>
       </c>
@@ -16219,7 +16220,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:61">
       <c r="A18" t="s">
         <v>111</v>
       </c>
@@ -16402,7 +16403,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:61">
       <c r="A19" t="s">
         <v>114</v>
       </c>
@@ -16585,7 +16586,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:61">
       <c r="A20" t="s">
         <v>115</v>
       </c>
@@ -16768,7 +16769,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:61">
       <c r="A21" t="s">
         <v>116</v>
       </c>
@@ -16951,7 +16952,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:61">
       <c r="A22" t="s">
         <v>117</v>
       </c>
@@ -17134,7 +17135,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:61">
       <c r="A23" t="s">
         <v>118</v>
       </c>
@@ -17317,7 +17318,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:61">
       <c r="A24" t="s">
         <v>119</v>
       </c>
@@ -17500,7 +17501,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:61">
       <c r="A25" t="s">
         <v>120</v>
       </c>
@@ -17683,7 +17684,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:61">
       <c r="A26" t="s">
         <v>121</v>
       </c>
@@ -17866,7 +17867,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:61">
       <c r="A27" t="s">
         <v>122</v>
       </c>
@@ -18049,7 +18050,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:61">
       <c r="A28" t="s">
         <v>123</v>
       </c>
@@ -18232,7 +18233,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:61">
       <c r="A29" t="s">
         <v>124</v>
       </c>
@@ -18415,7 +18416,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:61">
       <c r="A30" t="s">
         <v>125</v>
       </c>
@@ -18598,7 +18599,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:61">
       <c r="D31" s="11"/>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
@@ -18685,7 +18686,7 @@
       <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
@@ -18718,99 +18719,99 @@
     <col min="37" max="37" width="2.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:37">
       <c r="C1" s="6"/>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="18" t="s">
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="18" t="s">
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="24" t="s">
         <v>182</v>
       </c>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="18" t="s">
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="18"/>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="19"/>
-      <c r="AB1" s="18" t="s">
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="24"/>
+      <c r="AA1" s="25"/>
+      <c r="AB1" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="AC1" s="18"/>
-      <c r="AD1" s="18"/>
-      <c r="AE1" s="18"/>
-      <c r="AF1" s="18"/>
-      <c r="AG1" s="19"/>
+      <c r="AC1" s="24"/>
+      <c r="AD1" s="24"/>
+      <c r="AE1" s="24"/>
+      <c r="AF1" s="24"/>
+      <c r="AG1" s="25"/>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37">
       <c r="C2" s="1"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="22" t="s">
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22" t="s">
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="N2" s="22"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="22" t="s">
+      <c r="N2" s="21"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="22" t="s">
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="T2" s="22"/>
-      <c r="U2" s="23"/>
-      <c r="V2" s="22" t="s">
+      <c r="T2" s="21"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="W2" s="22"/>
-      <c r="X2" s="22"/>
-      <c r="Y2" s="22" t="s">
+      <c r="W2" s="21"/>
+      <c r="X2" s="21"/>
+      <c r="Y2" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="Z2" s="22"/>
-      <c r="AA2" s="23"/>
-      <c r="AB2" s="22" t="s">
+      <c r="Z2" s="21"/>
+      <c r="AA2" s="22"/>
+      <c r="AB2" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="AC2" s="22"/>
-      <c r="AD2" s="22"/>
-      <c r="AE2" s="22" t="s">
+      <c r="AC2" s="21"/>
+      <c r="AD2" s="21"/>
+      <c r="AE2" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="AF2" s="22"/>
-      <c r="AG2" s="23"/>
+      <c r="AF2" s="21"/>
+      <c r="AG2" s="22"/>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:37">
       <c r="B3" t="s">
         <v>26</v>
       </c>
@@ -18871,7 +18872,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:37">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -18902,7 +18903,7 @@
       <c r="J4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="18" t="s">
         <v>185</v>
       </c>
       <c r="L4" s="2" t="s">
@@ -18929,7 +18930,7 @@
       <c r="S4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="T4" s="25" t="s">
+      <c r="T4" s="19" t="s">
         <v>191</v>
       </c>
       <c r="U4" s="3" t="s">
@@ -18965,7 +18966,7 @@
       <c r="AE4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AF4" s="25" t="s">
+      <c r="AF4" s="19" t="s">
         <v>192</v>
       </c>
       <c r="AG4" s="3" t="s">
@@ -18981,7 +18982,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:37">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -19092,7 +19093,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:37">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -19203,7 +19204,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:37">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -19314,7 +19315,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:37">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -19425,7 +19426,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:37">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -19536,7 +19537,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:37">
       <c r="A10" t="s">
         <v>60</v>
       </c>
@@ -19647,7 +19648,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:37">
       <c r="A11" t="s">
         <v>114</v>
       </c>
@@ -19758,7 +19759,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:37">
       <c r="A12" t="s">
         <v>115</v>
       </c>
@@ -19869,7 +19870,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:37">
       <c r="A13" t="s">
         <v>116</v>
       </c>
@@ -19980,7 +19981,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:37">
       <c r="A14" t="s">
         <v>117</v>
       </c>
@@ -20091,7 +20092,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:37">
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
@@ -20124,20 +20125,20 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="D2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="J1:O1"/>
+    <mergeCell ref="P1:U1"/>
+    <mergeCell ref="V1:AA1"/>
+    <mergeCell ref="AB1:AG1"/>
     <mergeCell ref="V2:X2"/>
     <mergeCell ref="Y2:AA2"/>
     <mergeCell ref="AB2:AD2"/>
     <mergeCell ref="S2:U2"/>
     <mergeCell ref="AE2:AG2"/>
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="J1:O1"/>
-    <mergeCell ref="P1:U1"/>
-    <mergeCell ref="V1:AA1"/>
-    <mergeCell ref="AB1:AG1"/>
-    <mergeCell ref="D2:I2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="P2:R2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20149,7 +20150,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
populated 11 equations in full dynamics
</commit_message>
<xml_diff>
--- a/full dynamics.xlsx
+++ b/full dynamics.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/StephaneMagnan/Documents/GitHub/QWOP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86F7D37-93A9-3E48-A2CA-F001D78802D6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D6C9A0-CE37-0D4F-899F-DC89528DB6BC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="3" xr2:uid="{28E72DDC-E907-8543-92E7-F3D54FAF7A29}"/>
   </bookViews>
@@ -20,7 +20,6 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3587" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3550" uniqueCount="240">
   <si>
     <t>x</t>
   </si>
@@ -584,47 +583,185 @@
     <t>-m4*g*gamma4*np.sin(theta4l)+k4*(theta3l+phi4l-theta4l)+c4*(theta3ldot-theta4ldot)+fFl*(l4)*np.cos(theta4l)+fNl*(l4)*np.sin(theta4l)</t>
   </si>
   <si>
-    <t>Right Leg</t>
-  </si>
-  <si>
-    <t>m+2*m1+2*m2+2*m3+2*m4</t>
-  </si>
-  <si>
-    <t>-2*m1*gamma*np.cos(theta)-2*m2*gamma*np.cos(theta)+2*m3*(l-gamma)*np.cos(theta)+2*m4*(l-gamma)*np.cos(theta)</t>
-  </si>
-  <si>
-    <t>m1*gamma1*np.cos(theta1r)+m2*l1*np.cos(theta1r)</t>
-  </si>
-  <si>
-    <t>m1*gamma1*np.cos(theta1l)+m2*L1*np.cos(theta1l)</t>
-  </si>
-  <si>
-    <t>m3*(gamma3)*np.cos(theta3r)+m4*(l3)*np.cos(theta3r)</t>
-  </si>
-  <si>
-    <t>m3*(gamma3)*np.cos(theta3l)+m4*(l3)*np.cos(theta3l)</t>
-  </si>
-  <si>
-    <t>m2*gamma2*np.cos(thet2r)</t>
-  </si>
-  <si>
-    <t>m2*gamma2*np.cos(thet2l)</t>
-  </si>
-  <si>
-    <t>m4*gamma4*np.cos(thet4r)</t>
-  </si>
-  <si>
-    <t>m4*gamma4*np.cos(thet4l)</t>
-  </si>
-  <si>
-    <t>fFr+fFl-m1*gamma*thetadot**2*np.sin(theta)+m1*gamma1*thetadot1r**2*np.sin(theta1r)-m2*gamma*thetadot**2*np.sin(theta)+m2*l1*thetadot1r**2*np.sin(theta1r)+m2*gamma2*thetadot2r**2*np.sin(theta2r)+m3*(l-gamma)*thetadot**2*np.sin(theta)+m3*gamma3*thetadot3r**2*np.sin(theta3r)+m4*(l-gamma)*thetadot**2*np.sin(theta)+m4*l3*thetadot3r**2*np.sin(theta3r)+m4*gamma4*thetadot4r**2*np.sin(theta4r)-m1*gamma*thetadot**2*np.sin(theta)+m1*gamma1*thetadot1l**2*np.sin(theta1l)-m2*gamma*thetadot**2*np.sin(theta)+m2*l1*thetadot1l**2*np.sin(theta1l)+m2*gamma2*thetadot2l**2*np.sin(theta2l)+m3*(l-gamma)*thetadot**2*np.sin(theta)+m3*gamma3*thetadot3l**2*np.sin(theta3l)+m4*(l-gamma)*thetadot**2*np.sin(theta)+m4*l3*thetadot3l**2*np.sin(theta3l)+m4*gamma4*thetadot4l**2*np.sin(theta4l)</t>
+    <t>﻿m + 2*m1 + 2*m2 + 2*m3 + 2*m4</t>
+  </si>
+  <si>
+    <t>﻿-2*gamma*m1*cos(theta) - 2*gamma*m2*cos(theta) - 2*gamma*m3*cos(theta) - 2*gamma*m4*cos(theta) + 2*l*m3*cos(theta) + 2*l*m4*cos(theta)</t>
+  </si>
+  <si>
+    <t>﻿gamma1*m1*cos(theta1r) + l1*m2*cos(theta1r)</t>
+  </si>
+  <si>
+    <t>﻿gamma2*m2*cos(theta2r)</t>
+  </si>
+  <si>
+    <t>﻿gamma3*m3*cos(theta3r) + l3*m4*cos(theta3r)</t>
+  </si>
+  <si>
+    <t>﻿gamma4*m4*cos(theta4r)</t>
+  </si>
+  <si>
+    <t>﻿gamma1*m1*cos(theta1l) + l1*m2*cos(theta1l)</t>
+  </si>
+  <si>
+    <t>﻿gamma2*m2*cos(theta2l)</t>
+  </si>
+  <si>
+    <t>﻿gamma3*m3*cos(theta3l) + l3*m4*cos(theta3l)</t>
+  </si>
+  <si>
+    <t>﻿gamma4*m4*cos(theta4l)</t>
+  </si>
+  <si>
+    <t>﻿fFl + fFr - 2*gamma*m1*thetadot**2*sin(theta) - 2*gamma*m2*thetadot**2*sin(theta) - 2*gamma*m3*thetadot**2*sin(theta) - 2*gamma*m4*thetadot**2*sin(theta) + gamma1*m1*theta1ldot**2*sin(theta1l) + gamma1*m1*theta1rdot**2*sin(theta1r) + gamma2*m2*theta2ldot**2*sin(theta2l) + gamma2*m2*theta2rdot**2*sin(theta2r) + gamma3*m3*theta3ldot**2*sin(theta3l) + gamma3*m3*theta3rdot**2*sin(theta3r) + gamma4*m4*theta4ldot**2*sin(theta4l) + gamma4*m4*theta4rdot**2*sin(theta4r) + 2*l*m3*thetadot**2*sin(theta) + 2*l*m4*thetadot**2*sin(theta) + l1*m2*theta1ldot**2*sin(theta1l) + l1*m2*theta1rdot**2*sin(theta1r) + l3*m4*theta3ldot**2*sin(theta3l) + l3*m4*theta3rdot**2*sin(theta3r)</t>
+  </si>
+  <si>
+    <t>﻿-2*gamma*m1*sin(theta) - 2*gamma*m2*sin(theta) - 2*gamma*m3*sin(theta) - 2*gamma*m4*sin(theta) + 2*l*m3*sin(theta) + 2*l*m4*sin(theta)</t>
+  </si>
+  <si>
+    <t>﻿gamma1*m1*sin(theta1r) + l1*m2*sin(theta1r)</t>
+  </si>
+  <si>
+    <t>﻿gamma2*m2*sin(theta2r)</t>
+  </si>
+  <si>
+    <t>﻿gamma3*m3*sin(theta3r) + l3*m4*sin(theta3r)</t>
+  </si>
+  <si>
+    <t>﻿gamma4*m4*sin(theta4r)</t>
+  </si>
+  <si>
+    <t>﻿gamma1*m1*sin(theta1l) + l1*m2*sin(theta1l)</t>
+  </si>
+  <si>
+    <t>﻿gamma2*m2*sin(theta2l)</t>
+  </si>
+  <si>
+    <t>﻿gamma3*m3*sin(theta3l) + l3*m4*sin(theta3l)</t>
+  </si>
+  <si>
+    <t>﻿gamma4*m4*sin(theta4l)</t>
+  </si>
+  <si>
+    <t>﻿fNl + fNr - g*m - 2*g*m1 - 2*g*m2 - 2*g*m3 - 2*g*m4 + 2*gamma*m1*thetadot**2*cos(theta) + 2*gamma*m2*thetadot**2*cos(theta) + 2*gamma*m3*thetadot**2*cos(theta) + 2*gamma*m4*thetadot**2*cos(theta) - gamma1*m1*theta1ldot**2*cos(theta1l) - gamma1*m1*theta1rdot**2*cos(theta1r) - gamma2*m2*theta2ldot**2*cos(theta2l) - gamma2*m2*theta2rdot**2*cos(theta2r) - gamma3*m3*theta3ldot**2*cos(theta3l) - gamma3*m3*theta3rdot**2*cos(theta3r) - gamma4*m4*theta4ldot**2*cos(theta4l) - gamma4*m4*theta4rdot**2*cos(theta4r) - 2*l*m3*thetadot**2*cos(theta) - 2*l*m4*thetadot**2*cos(theta) - l1*m2*theta1ldot**2*cos(theta1l) - l1*m2*theta1rdot**2*cos(theta1r) - l3*m4*theta3ldot**2*cos(theta3l) - l3*m4*theta3rdot**2*cos(theta3r)</t>
+  </si>
+  <si>
+    <t>﻿I + 2*gamma**2*m1*sin(theta)**2 + 2*gamma**2*m1*cos(theta)**2 + 2*gamma**2*m2*sin(theta)**2 + 2*gamma**2*m2*cos(theta)**2 + 2*gamma**2*m3*sin(theta)**2 + 2*gamma**2*m3*cos(theta)**2 + 2*gamma**2*m4*sin(theta)**2 + 2*gamma**2*m4*cos(theta)**2 - 4*gamma*l*m3*sin(theta)**2 - 4*gamma*l*m3*cos(theta)**2 - 4*gamma*l*m4*sin(theta)**2 - 4*gamma*l*m4*cos(theta)**2 + 2*l**2*m3*sin(theta)**2 + 2*l**2*m3*cos(theta)**2 + 2*l**2*m4*sin(theta)**2 + 2*l**2*m4*cos(theta)**2</t>
+  </si>
+  <si>
+    <t>﻿-gamma*gamma1*m1*sin(theta)*sin(theta1r) - gamma*gamma1*m1*cos(theta)*cos(theta1r) - gamma*l1*m2*sin(theta)*sin(theta1r) - gamma*l1*m2*cos(theta)*cos(theta1r)</t>
+  </si>
+  <si>
+    <t>﻿-gamma*gamma2*m2*sin(theta)*sin(theta2r) - gamma*gamma2*m2*cos(theta)*cos(theta2r)</t>
+  </si>
+  <si>
+    <t>﻿-gamma*gamma3*m3*sin(theta)*sin(theta3r) - gamma*gamma3*m3*cos(theta)*cos(theta3r) - gamma*l3*m4*sin(theta)*sin(theta3r) - gamma*l3*m4*cos(theta)*cos(theta3r) + gamma3*l*m3*sin(theta)*sin(theta3r) + gamma3*l*m3*cos(theta)*cos(theta3r) + l*l3*m4*sin(theta)*sin(theta3r) + l*l3*m4*cos(theta)*cos(theta3r)</t>
+  </si>
+  <si>
+    <t>﻿-gamma*gamma4*m4*sin(theta)*sin(theta4r) - gamma*gamma4*m4*cos(theta)*cos(theta4r) + gamma4*l*m4*sin(theta)*sin(theta4r) + gamma4*l*m4*cos(theta)*cos(theta4r)</t>
+  </si>
+  <si>
+    <t>﻿-gamma*gamma1*m1*sin(theta)*sin(theta1l) - gamma*gamma1*m1*cos(theta)*cos(theta1l) - gamma*l1*m2*sin(theta)*sin(theta1l) - gamma*l1*m2*cos(theta)*cos(theta1l)</t>
+  </si>
+  <si>
+    <t>﻿-gamma*gamma2*m2*sin(theta)*sin(theta2l) - gamma*gamma2*m2*cos(theta)*cos(theta2l)</t>
+  </si>
+  <si>
+    <t>﻿-gamma*gamma3*m3*sin(theta)*sin(theta3l) - gamma*gamma3*m3*cos(theta)*cos(theta3l) - gamma*l3*m4*sin(theta)*sin(theta3l) - gamma*l3*m4*cos(theta)*cos(theta3l) + gamma3*l*m3*sin(theta)*sin(theta3l) + gamma3*l*m3*cos(theta)*cos(theta3l) + l*l3*m4*sin(theta)*sin(theta3l) + l*l3*m4*cos(theta)*cos(theta3l)</t>
+  </si>
+  <si>
+    <t>﻿-gamma*gamma4*m4*sin(theta)*sin(theta4l) - gamma*gamma4*m4*cos(theta)*cos(theta4l) + gamma4*l*m4*sin(theta)*sin(theta4l) + gamma4*l*m4*cos(theta)*cos(theta4l)</t>
+  </si>
+  <si>
+    <t>﻿c1*theta1ldot + c1*theta1rdot - 2*c1*thetadot + c3*theta3ldot + c3*theta3rdot - 2*c3*thetadot - fFl*gamma*cos(theta) + fFl*l*cos(theta) - fFr*gamma*cos(theta) + fFr*l*cos(theta) - fNl*gamma*sin(theta) + fNl*l*sin(theta) - fNr*gamma*sin(theta) + fNr*l*sin(theta) + 2*g*gamma*m1*sin(theta) + 2*g*gamma*m2*sin(theta) + 2*g*gamma*m3*sin(theta) + 2*g*gamma*m4*sin(theta) - 2*g*l*m3*sin(theta) - 2*g*l*m4*sin(theta) + gamma*gamma1*m1*theta1ldot**2*sin(theta)*cos(theta1l) - gamma*gamma1*m1*theta1ldot**2*sin(theta1l)*cos(theta) + gamma*gamma1*m1*theta1rdot**2*sin(theta)*cos(theta1r) - gamma*gamma1*m1*theta1rdot**2*sin(theta1r)*cos(theta) + gamma*gamma2*m2*theta2ldot**2*sin(theta)*cos(theta2l) - gamma*gamma2*m2*theta2ldot**2*sin(theta2l)*cos(theta) + gamma*gamma2*m2*theta2rdot**2*sin(theta)*cos(theta2r) - gamma*gamma2*m2*theta2rdot**2*sin(theta2r)*cos(theta) + gamma*gamma3*m3*theta3ldot**2*sin(theta)*cos(theta3l) - gamma*gamma3*m3*theta3ldot**2*sin(theta3l)*cos(theta) + gamma*gamma3*m3*theta3rdot**2*sin(theta)*cos(theta3r) - gamma*gamma3*m3*theta3rdot**2*sin(theta3r)*cos(theta) + gamma*gamma4*m4*theta4ldot**2*sin(theta)*cos(theta4l) - gamma*gamma4*m4*theta4ldot**2*sin(theta4l)*cos(theta) + gamma*gamma4*m4*theta4rdot**2*sin(theta)*cos(theta4r) - gamma*gamma4*m4*theta4rdot**2*sin(theta4r)*cos(theta) + gamma*l1*m2*theta1ldot**2*sin(theta)*cos(theta1l) - gamma*l1*m2*theta1ldot**2*sin(theta1l)*cos(theta) + gamma*l1*m2*theta1rdot**2*sin(theta)*cos(theta1r) - gamma*l1*m2*theta1rdot**2*sin(theta1r)*cos(theta) + gamma*l3*m4*theta3ldot**2*sin(theta)*cos(theta3l) - gamma*l3*m4*theta3ldot**2*sin(theta3l)*cos(theta) + gamma*l3*m4*theta3rdot**2*sin(theta)*cos(theta3r) - gamma*l3*m4*theta3rdot**2*sin(theta3r)*cos(theta) - gamma3*l*m3*theta3ldot**2*sin(theta)*cos(theta3l) + gamma3*l*m3*theta3ldot**2*sin(theta3l)*cos(theta) - gamma3*l*m3*theta3rdot**2*sin(theta)*cos(theta3r) + gamma3*l*m3*theta3rdot**2*sin(theta3r)*cos(theta) - gamma4*l*m4*theta4ldot**2*sin(theta)*cos(theta4l) + gamma4*l*m4*theta4ldot**2*sin(theta4l)*cos(theta) - gamma4*l*m4*theta4rdot**2*sin(theta)*cos(theta4r) + gamma4*l*m4*theta4rdot**2*sin(theta4r)*cos(theta) - k1*phi1l - k1*phi1r - 2*k1*theta + k1*theta1l + k1*theta1r - k3*phi3l - k3*phi3r - 2*k3*theta + k3*theta3l + k3*theta3r - l*l3*m4*theta3ldot**2*sin(theta)*cos(theta3l) + l*l3*m4*theta3ldot**2*sin(theta3l)*cos(theta) - l*l3*m4*theta3rdot**2*sin(theta)*cos(theta3r) + l*l3*m4*theta3rdot**2*sin(theta3r)*cos(theta)</t>
+  </si>
+  <si>
+    <t>﻿I1 + gamma1**2*m1*sin(theta1r)**2 + gamma1**2*m1*cos(theta1r)**2 + l1**2*m2*sin(theta1r)**2 + l1**2*m2*cos(theta1r)**2</t>
+  </si>
+  <si>
+    <t>﻿gamma2*l1*m2*sin(theta1r)*sin(theta2r) + gamma2*l1*m2*cos(theta1r)*cos(theta2r)</t>
+  </si>
+  <si>
+    <t>﻿-c1*theta1rdot + c1*thetadot - c2*theta1rdot + c2*theta2rdot - g*gamma1*m1*sin(theta1r) - g*l1*m2*sin(theta1r) - gamma*gamma1*m1*thetadot**2*sin(theta)*cos(theta1r) + gamma*gamma1*m1*thetadot**2*sin(theta1r)*cos(theta) - gamma*l1*m2*thetadot**2*sin(theta)*cos(theta1r) + gamma*l1*m2*thetadot**2*sin(theta1r)*cos(theta) - gamma2*l1*m2*theta2rdot**2*sin(theta1r)*cos(theta2r) + gamma2*l1*m2*theta2rdot**2*sin(theta2r)*cos(theta1r) + k1*phi1r + k1*theta - k1*theta1r - k2*phi2r - k2*theta1r + k2*theta2r</t>
+  </si>
+  <si>
+    <t>﻿I2 + gamma2**2*m2*sin(theta2r)**2 + gamma2**2*m2*cos(theta2r)**2</t>
+  </si>
+  <si>
+    <t>﻿c2*theta1rdot - c2*theta2rdot - g*gamma2*m2*sin(theta2r) - gamma*gamma2*m2*thetadot**2*sin(theta)*cos(theta2r) + gamma*gamma2*m2*thetadot**2*sin(theta2r)*cos(theta) + gamma2*l1*m2*theta1rdot**2*sin(theta1r)*cos(theta2r) - gamma2*l1*m2*theta1rdot**2*sin(theta2r)*cos(theta1r) + k2*phi2r + k2*theta1r - k2*theta2r</t>
+  </si>
+  <si>
+    <t>﻿I3 + gamma3**2*m3*sin(theta3r)**2 + gamma3**2*m3*cos(theta3r)**2 + l3**2*m4*sin(theta3r)**2 + l3**2*m4*cos(theta3r)**2</t>
+  </si>
+  <si>
+    <t>﻿gamma4*l3*m4*sin(theta3r)*sin(theta4r) + gamma4*l3*m4*cos(theta3r)*cos(theta4r)</t>
+  </si>
+  <si>
+    <t>﻿-c3*theta3rdot + c3*thetadot - c4*theta3rdot + c4*theta4rdot + fFr*l3*cos(theta3r) + fNr*l3*sin(theta3r) - g*gamma3*m3*sin(theta3r) - g*l3*m4*sin(theta3r) - gamma*gamma3*m3*thetadot**2*sin(theta)*cos(theta3r) + gamma*gamma3*m3*thetadot**2*sin(theta3r)*cos(theta) - gamma*l3*m4*thetadot**2*sin(theta)*cos(theta3r) + gamma*l3*m4*thetadot**2*sin(theta3r)*cos(theta) + gamma3*l*m3*thetadot**2*sin(theta)*cos(theta3r) - gamma3*l*m3*thetadot**2*sin(theta3r)*cos(theta) - gamma4*l3*m4*theta4rdot**2*sin(theta3r)*cos(theta4r) + gamma4*l3*m4*theta4rdot**2*sin(theta4r)*cos(theta3r) + k3*phi3r + k3*theta - k3*theta3r - k4*phi4r - k4*theta3r + k4*theta4r + l*l3*m4*thetadot**2*sin(theta)*cos(theta3r) - l*l3*m4*thetadot**2*sin(theta3r)*cos(theta)</t>
+  </si>
+  <si>
+    <t>﻿I4 + gamma4**2*m4*sin(theta4r)**2 + gamma4**2*m4*cos(theta4r)**2</t>
+  </si>
+  <si>
+    <t>﻿c4*theta3rdot - c4*theta4rdot + fFr*l4*cos(theta4r) + fNr*l4*sin(theta4r) - g*gamma4*m4*sin(theta4r) - gamma*gamma4*m4*thetadot**2*sin(theta)*cos(theta4r) + gamma*gamma4*m4*thetadot**2*sin(theta4r)*cos(theta) + gamma4*l*m4*thetadot**2*sin(theta)*cos(theta4r) - gamma4*l*m4*thetadot**2*sin(theta4r)*cos(theta) + gamma4*l3*m4*theta3rdot**2*sin(theta3r)*cos(theta4r) - gamma4*l3*m4*theta3rdot**2*sin(theta4r)*cos(theta3r) + k4*phi4r + k4*theta3r - k4*theta4r</t>
+  </si>
+  <si>
+    <t>﻿I1 + gamma1**2*m1*sin(theta1l)**2 + gamma1**2*m1*cos(theta1l)**2 + l1**2*m2*sin(theta1l)**2 + l1**2*m2*cos(theta1l)**2</t>
+  </si>
+  <si>
+    <t>﻿gamma2*l1*m2*sin(theta1l)*sin(theta2l) + gamma2*l1*m2*cos(theta1l)*cos(theta2l)</t>
+  </si>
+  <si>
+    <t>﻿-c1*theta1ldot + c1*thetadot - c2*theta1ldot + c2*theta2ldot - g*gamma1*m1*sin(theta1l) - g*l1*m2*sin(theta1l) - gamma*gamma1*m1*thetadot**2*sin(theta)*cos(theta1l) + gamma*gamma1*m1*thetadot**2*sin(theta1l)*cos(theta) - gamma*l1*m2*thetadot**2*sin(theta)*cos(theta1l) + gamma*l1*m2*thetadot**2*sin(theta1l)*cos(theta) - gamma2*l1*m2*theta2ldot**2*sin(theta1l)*cos(theta2l) + gamma2*l1*m2*theta2ldot**2*sin(theta2l)*cos(theta1l) + k1*phi1l + k1*theta - k1*theta1l - k2*phi2l - k2*theta1l + k2*theta2l</t>
+  </si>
+  <si>
+    <t>﻿I2 + gamma2**2*m2*sin(theta2l)**2 + gamma2**2*m2*cos(theta2l)**2</t>
+  </si>
+  <si>
+    <t>﻿c2*theta1ldot - c2*theta2ldot - g*gamma2*m2*sin(theta2l) - gamma*gamma2*m2*thetadot**2*sin(theta)*cos(theta2l) + gamma*gamma2*m2*thetadot**2*sin(theta2l)*cos(theta) + gamma2*l1*m2*theta1ldot**2*sin(theta1l)*cos(theta2l) - gamma2*l1*m2*theta1ldot**2*sin(theta2l)*cos(theta1l) + k2*phi2l + k2*theta1l - k2*theta2l</t>
+  </si>
+  <si>
+    <t>﻿I3 + gamma3**2*m3*sin(theta3l)**2 + gamma3**2*m3*cos(theta3l)**2 + l3**2*m4*sin(theta3l)**2 + l3**2*m4*cos(theta3l)**2</t>
+  </si>
+  <si>
+    <t>﻿gamma4*l3*m4*sin(theta3l)*sin(theta4l) + gamma4*l3*m4*cos(theta3l)*cos(theta4l)</t>
+  </si>
+  <si>
+    <t>﻿-c3*theta3ldot + c3*thetadot - c4*theta3ldot + c4*theta4ldot + fFl*l3*cos(theta3l) + fNl*l3*sin(theta3l) - g*gamma3*m3*sin(theta3l) - g*l3*m4*sin(theta3l) - gamma*gamma3*m3*thetadot**2*sin(theta)*cos(theta3l) + gamma*gamma3*m3*thetadot**2*sin(theta3l)*cos(theta) - gamma*l3*m4*thetadot**2*sin(theta)*cos(theta3l) + gamma*l3*m4*thetadot**2*sin(theta3l)*cos(theta) + gamma3*l*m3*thetadot**2*sin(theta)*cos(theta3l) - gamma3*l*m3*thetadot**2*sin(theta3l)*cos(theta) - gamma4*l3*m4*theta4ldot**2*sin(theta3l)*cos(theta4l) + gamma4*l3*m4*theta4ldot**2*sin(theta4l)*cos(theta3l) + k3*phi3l + k3*theta - k3*theta3l - k4*phi4l - k4*theta3l + k4*theta4l + l*l3*m4*thetadot**2*sin(theta)*cos(theta3l) - l*l3*m4*thetadot**2*sin(theta3l)*cos(theta)</t>
+  </si>
+  <si>
+    <t>﻿I4 + gamma4**2*m4*sin(theta4l)**2 + gamma4**2*m4*cos(theta4l)**2</t>
+  </si>
+  <si>
+    <t>﻿c4*theta3ldot - c4*theta4ldot + fFl*l4*cos(theta4l) + fNl*l4*sin(theta4l) - g*gamma4*m4*sin(theta4l) - gamma*gamma4*m4*thetadot**2*sin(theta)*cos(theta4l) + gamma*gamma4*m4*thetadot**2*sin(theta4l)*cos(theta) + gamma4*l*m4*thetadot**2*sin(theta)*cos(theta4l) - gamma4*l*m4*thetadot**2*sin(theta4l)*cos(theta) + gamma4*l3*m4*theta3ldot**2*sin(theta3l)*cos(theta4l) - gamma4*l3*m4*theta3ldot**2*sin(theta4l)*cos(theta3l) + k4*phi4l + k4*theta3l - k4*theta4l</t>
+  </si>
+  <si>
+    <t>RIGHT ARM</t>
+  </si>
+  <si>
+    <t>PROXIMAL</t>
+  </si>
+  <si>
+    <t>DISTAL</t>
+  </si>
+  <si>
+    <t>RIGHT LEG</t>
+  </si>
+  <si>
+    <t>LEFT ARM</t>
+  </si>
+  <si>
+    <t>LEFT LEG</t>
+  </si>
+  <si>
+    <t>BODY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -636,13 +773,6 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -745,7 +875,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -766,8 +896,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -775,15 +912,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1109,7 +1237,7 @@
       <selection pane="bottomRight" activeCell="AZ30" sqref="AZ30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
@@ -1182,167 +1310,167 @@
     <col min="69" max="69" width="2.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69">
+    <row r="1" spans="1:69" x14ac:dyDescent="0.2">
       <c r="C1" s="6"/>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="23" t="s">
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
-      <c r="S1" s="24"/>
-      <c r="T1" s="24"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="23" t="s">
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="W1" s="24"/>
-      <c r="X1" s="24"/>
-      <c r="Y1" s="24"/>
-      <c r="Z1" s="24"/>
-      <c r="AA1" s="24"/>
-      <c r="AB1" s="24"/>
-      <c r="AC1" s="24"/>
-      <c r="AD1" s="24"/>
-      <c r="AE1" s="24"/>
-      <c r="AF1" s="24"/>
-      <c r="AG1" s="24"/>
-      <c r="AH1" s="24"/>
-      <c r="AI1" s="24"/>
-      <c r="AJ1" s="24"/>
-      <c r="AK1" s="25"/>
-      <c r="AL1" s="23" t="s">
+      <c r="W1" s="18"/>
+      <c r="X1" s="18"/>
+      <c r="Y1" s="18"/>
+      <c r="Z1" s="18"/>
+      <c r="AA1" s="18"/>
+      <c r="AB1" s="18"/>
+      <c r="AC1" s="18"/>
+      <c r="AD1" s="18"/>
+      <c r="AE1" s="18"/>
+      <c r="AF1" s="18"/>
+      <c r="AG1" s="18"/>
+      <c r="AH1" s="18"/>
+      <c r="AI1" s="18"/>
+      <c r="AJ1" s="18"/>
+      <c r="AK1" s="19"/>
+      <c r="AL1" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="AM1" s="24"/>
-      <c r="AN1" s="24"/>
-      <c r="AO1" s="24"/>
-      <c r="AP1" s="24"/>
-      <c r="AQ1" s="24"/>
-      <c r="AR1" s="24"/>
-      <c r="AS1" s="24"/>
-      <c r="AT1" s="24"/>
-      <c r="AU1" s="24"/>
-      <c r="AV1" s="24"/>
-      <c r="AW1" s="25"/>
-      <c r="AX1" s="23" t="s">
+      <c r="AM1" s="18"/>
+      <c r="AN1" s="18"/>
+      <c r="AO1" s="18"/>
+      <c r="AP1" s="18"/>
+      <c r="AQ1" s="18"/>
+      <c r="AR1" s="18"/>
+      <c r="AS1" s="18"/>
+      <c r="AT1" s="18"/>
+      <c r="AU1" s="18"/>
+      <c r="AV1" s="18"/>
+      <c r="AW1" s="19"/>
+      <c r="AX1" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="AY1" s="24"/>
-      <c r="AZ1" s="24"/>
-      <c r="BA1" s="24"/>
-      <c r="BB1" s="24"/>
-      <c r="BC1" s="24"/>
-      <c r="BD1" s="24"/>
-      <c r="BE1" s="24"/>
-      <c r="BF1" s="24"/>
-      <c r="BG1" s="24"/>
-      <c r="BH1" s="24"/>
-      <c r="BI1" s="24"/>
-      <c r="BJ1" s="24"/>
-      <c r="BK1" s="24"/>
-      <c r="BL1" s="24"/>
-      <c r="BM1" s="25"/>
+      <c r="AY1" s="18"/>
+      <c r="AZ1" s="18"/>
+      <c r="BA1" s="18"/>
+      <c r="BB1" s="18"/>
+      <c r="BC1" s="18"/>
+      <c r="BD1" s="18"/>
+      <c r="BE1" s="18"/>
+      <c r="BF1" s="18"/>
+      <c r="BG1" s="18"/>
+      <c r="BH1" s="18"/>
+      <c r="BI1" s="18"/>
+      <c r="BJ1" s="18"/>
+      <c r="BK1" s="18"/>
+      <c r="BL1" s="18"/>
+      <c r="BM1" s="19"/>
     </row>
-    <row r="2" spans="1:69">
+    <row r="2" spans="1:69" x14ac:dyDescent="0.2">
       <c r="C2" s="1"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="20" t="s">
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21" t="s">
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="21"/>
-      <c r="T2" s="21"/>
-      <c r="U2" s="22"/>
-      <c r="V2" s="20" t="s">
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="22"/>
+      <c r="U2" s="23"/>
+      <c r="V2" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="W2" s="21"/>
-      <c r="X2" s="21"/>
-      <c r="Y2" s="21"/>
-      <c r="Z2" s="21"/>
-      <c r="AA2" s="21"/>
-      <c r="AB2" s="21" t="s">
+      <c r="W2" s="22"/>
+      <c r="X2" s="22"/>
+      <c r="Y2" s="22"/>
+      <c r="Z2" s="22"/>
+      <c r="AA2" s="22"/>
+      <c r="AB2" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="AC2" s="21"/>
-      <c r="AD2" s="21"/>
-      <c r="AE2" s="21"/>
-      <c r="AF2" s="21"/>
-      <c r="AG2" s="21"/>
-      <c r="AH2" s="21" t="s">
+      <c r="AC2" s="22"/>
+      <c r="AD2" s="22"/>
+      <c r="AE2" s="22"/>
+      <c r="AF2" s="22"/>
+      <c r="AG2" s="22"/>
+      <c r="AH2" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="AI2" s="21"/>
-      <c r="AJ2" s="21"/>
-      <c r="AK2" s="22"/>
-      <c r="AL2" s="20" t="s">
+      <c r="AI2" s="22"/>
+      <c r="AJ2" s="22"/>
+      <c r="AK2" s="23"/>
+      <c r="AL2" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="AM2" s="21"/>
-      <c r="AN2" s="21"/>
-      <c r="AO2" s="21"/>
-      <c r="AP2" s="21"/>
-      <c r="AQ2" s="21"/>
-      <c r="AR2" s="21" t="s">
+      <c r="AM2" s="22"/>
+      <c r="AN2" s="22"/>
+      <c r="AO2" s="22"/>
+      <c r="AP2" s="22"/>
+      <c r="AQ2" s="22"/>
+      <c r="AR2" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="AS2" s="21"/>
-      <c r="AT2" s="21"/>
-      <c r="AU2" s="21"/>
-      <c r="AV2" s="21"/>
-      <c r="AW2" s="22"/>
-      <c r="AX2" s="20" t="s">
+      <c r="AS2" s="22"/>
+      <c r="AT2" s="22"/>
+      <c r="AU2" s="22"/>
+      <c r="AV2" s="22"/>
+      <c r="AW2" s="23"/>
+      <c r="AX2" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="AY2" s="21"/>
-      <c r="AZ2" s="21"/>
-      <c r="BA2" s="21"/>
-      <c r="BB2" s="21"/>
-      <c r="BC2" s="21"/>
-      <c r="BD2" s="21" t="s">
+      <c r="AY2" s="22"/>
+      <c r="AZ2" s="22"/>
+      <c r="BA2" s="22"/>
+      <c r="BB2" s="22"/>
+      <c r="BC2" s="22"/>
+      <c r="BD2" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="BE2" s="21"/>
-      <c r="BF2" s="21"/>
-      <c r="BG2" s="21"/>
-      <c r="BH2" s="21"/>
-      <c r="BI2" s="21"/>
-      <c r="BJ2" s="21" t="s">
+      <c r="BE2" s="22"/>
+      <c r="BF2" s="22"/>
+      <c r="BG2" s="22"/>
+      <c r="BH2" s="22"/>
+      <c r="BI2" s="22"/>
+      <c r="BJ2" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="BK2" s="21"/>
-      <c r="BL2" s="21"/>
-      <c r="BM2" s="22"/>
+      <c r="BK2" s="22"/>
+      <c r="BL2" s="22"/>
+      <c r="BM2" s="23"/>
     </row>
-    <row r="3" spans="1:69">
+    <row r="3" spans="1:69" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>26</v>
       </c>
@@ -1475,7 +1603,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:69">
+    <row r="4" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -1681,7 +1809,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:69">
+    <row r="5" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -1888,7 +2016,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:69">
+    <row r="6" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -2095,7 +2223,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:69">
+    <row r="7" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -2302,7 +2430,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:69">
+    <row r="8" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -2509,7 +2637,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:69">
+    <row r="9" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -2716,7 +2844,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:69">
+    <row r="10" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>60</v>
       </c>
@@ -2923,7 +3051,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:69">
+    <row r="11" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>104</v>
       </c>
@@ -3130,7 +3258,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:69">
+    <row r="12" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>105</v>
       </c>
@@ -3337,7 +3465,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:69">
+    <row r="13" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>106</v>
       </c>
@@ -3544,7 +3672,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:69">
+    <row r="14" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>107</v>
       </c>
@@ -3751,7 +3879,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:69">
+    <row r="15" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>108</v>
       </c>
@@ -3958,7 +4086,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:69">
+    <row r="16" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>109</v>
       </c>
@@ -4165,7 +4293,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:69">
+    <row r="17" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>110</v>
       </c>
@@ -4372,7 +4500,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:69">
+    <row r="18" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>111</v>
       </c>
@@ -4579,7 +4707,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:69">
+    <row r="19" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>112</v>
       </c>
@@ -4786,7 +4914,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:69">
+    <row r="20" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>113</v>
       </c>
@@ -4993,7 +5121,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:69">
+    <row r="21" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>114</v>
       </c>
@@ -5200,7 +5328,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:69">
+    <row r="22" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>115</v>
       </c>
@@ -5407,7 +5535,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:69">
+    <row r="23" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>116</v>
       </c>
@@ -5614,7 +5742,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:69">
+    <row r="24" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>117</v>
       </c>
@@ -5821,7 +5949,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:69">
+    <row r="25" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>118</v>
       </c>
@@ -6028,7 +6156,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:69">
+    <row r="26" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>119</v>
       </c>
@@ -6235,7 +6363,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:69">
+    <row r="27" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>120</v>
       </c>
@@ -6442,7 +6570,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:69">
+    <row r="28" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>121</v>
       </c>
@@ -6649,7 +6777,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:69">
+    <row r="29" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>122</v>
       </c>
@@ -6856,7 +6984,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:69">
+    <row r="30" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>123</v>
       </c>
@@ -7063,7 +7191,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:69">
+    <row r="31" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>124</v>
       </c>
@@ -7270,7 +7398,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:69">
+    <row r="32" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>125</v>
       </c>
@@ -7477,7 +7605,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:69">
+    <row r="33" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>126</v>
       </c>
@@ -7684,7 +7812,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:69">
+    <row r="34" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>127</v>
       </c>
@@ -7891,7 +8019,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:69">
+    <row r="35" spans="1:69" x14ac:dyDescent="0.2">
       <c r="D35" s="11"/>
       <c r="E35" s="11"/>
       <c r="F35" s="11"/>
@@ -7956,11 +8084,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="J1:U1"/>
-    <mergeCell ref="J2:O2"/>
-    <mergeCell ref="P2:U2"/>
-    <mergeCell ref="D2:I2"/>
     <mergeCell ref="AL2:AQ2"/>
     <mergeCell ref="AR2:AW2"/>
     <mergeCell ref="AX2:BC2"/>
@@ -7972,6 +8095,11 @@
     <mergeCell ref="V2:AA2"/>
     <mergeCell ref="AB2:AG2"/>
     <mergeCell ref="AL1:AW1"/>
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="J1:U1"/>
+    <mergeCell ref="J2:O2"/>
+    <mergeCell ref="P2:U2"/>
+    <mergeCell ref="D2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7988,7 +8116,7 @@
       <selection pane="bottomRight" activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
@@ -8053,147 +8181,147 @@
     <col min="61" max="61" width="2.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61">
+    <row r="1" spans="1:61" x14ac:dyDescent="0.2">
       <c r="C1" s="6"/>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="23" t="s">
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
-      <c r="S1" s="24"/>
-      <c r="T1" s="24"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="23" t="s">
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="W1" s="24"/>
-      <c r="X1" s="24"/>
-      <c r="Y1" s="24"/>
-      <c r="Z1" s="24"/>
-      <c r="AA1" s="24"/>
-      <c r="AB1" s="24"/>
-      <c r="AC1" s="24"/>
-      <c r="AD1" s="24"/>
-      <c r="AE1" s="24"/>
-      <c r="AF1" s="24"/>
-      <c r="AG1" s="25"/>
-      <c r="AH1" s="23" t="s">
+      <c r="W1" s="18"/>
+      <c r="X1" s="18"/>
+      <c r="Y1" s="18"/>
+      <c r="Z1" s="18"/>
+      <c r="AA1" s="18"/>
+      <c r="AB1" s="18"/>
+      <c r="AC1" s="18"/>
+      <c r="AD1" s="18"/>
+      <c r="AE1" s="18"/>
+      <c r="AF1" s="18"/>
+      <c r="AG1" s="19"/>
+      <c r="AH1" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="AI1" s="24"/>
-      <c r="AJ1" s="24"/>
-      <c r="AK1" s="24"/>
-      <c r="AL1" s="24"/>
-      <c r="AM1" s="24"/>
-      <c r="AN1" s="24"/>
-      <c r="AO1" s="24"/>
-      <c r="AP1" s="24"/>
-      <c r="AQ1" s="24"/>
-      <c r="AR1" s="24"/>
-      <c r="AS1" s="25"/>
-      <c r="AT1" s="23" t="s">
+      <c r="AI1" s="18"/>
+      <c r="AJ1" s="18"/>
+      <c r="AK1" s="18"/>
+      <c r="AL1" s="18"/>
+      <c r="AM1" s="18"/>
+      <c r="AN1" s="18"/>
+      <c r="AO1" s="18"/>
+      <c r="AP1" s="18"/>
+      <c r="AQ1" s="18"/>
+      <c r="AR1" s="18"/>
+      <c r="AS1" s="19"/>
+      <c r="AT1" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="AU1" s="24"/>
-      <c r="AV1" s="24"/>
-      <c r="AW1" s="24"/>
-      <c r="AX1" s="24"/>
-      <c r="AY1" s="24"/>
-      <c r="AZ1" s="24"/>
-      <c r="BA1" s="24"/>
-      <c r="BB1" s="24"/>
-      <c r="BC1" s="24"/>
-      <c r="BD1" s="24"/>
-      <c r="BE1" s="25"/>
+      <c r="AU1" s="18"/>
+      <c r="AV1" s="18"/>
+      <c r="AW1" s="18"/>
+      <c r="AX1" s="18"/>
+      <c r="AY1" s="18"/>
+      <c r="AZ1" s="18"/>
+      <c r="BA1" s="18"/>
+      <c r="BB1" s="18"/>
+      <c r="BC1" s="18"/>
+      <c r="BD1" s="18"/>
+      <c r="BE1" s="19"/>
     </row>
-    <row r="2" spans="1:61">
+    <row r="2" spans="1:61" x14ac:dyDescent="0.2">
       <c r="C2" s="1"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="20" t="s">
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21" t="s">
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="21"/>
-      <c r="T2" s="21"/>
-      <c r="U2" s="22"/>
-      <c r="V2" s="20" t="s">
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="22"/>
+      <c r="U2" s="23"/>
+      <c r="V2" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="W2" s="21"/>
-      <c r="X2" s="21"/>
-      <c r="Y2" s="21"/>
-      <c r="Z2" s="21"/>
-      <c r="AA2" s="21"/>
-      <c r="AB2" s="21" t="s">
+      <c r="W2" s="22"/>
+      <c r="X2" s="22"/>
+      <c r="Y2" s="22"/>
+      <c r="Z2" s="22"/>
+      <c r="AA2" s="22"/>
+      <c r="AB2" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="AC2" s="21"/>
-      <c r="AD2" s="21"/>
-      <c r="AE2" s="21"/>
-      <c r="AF2" s="21"/>
+      <c r="AC2" s="22"/>
+      <c r="AD2" s="22"/>
+      <c r="AE2" s="22"/>
+      <c r="AF2" s="22"/>
       <c r="AG2" s="17"/>
-      <c r="AH2" s="20" t="s">
+      <c r="AH2" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="AI2" s="21"/>
-      <c r="AJ2" s="21"/>
-      <c r="AK2" s="21"/>
-      <c r="AL2" s="21"/>
-      <c r="AM2" s="21"/>
-      <c r="AN2" s="21" t="s">
+      <c r="AI2" s="22"/>
+      <c r="AJ2" s="22"/>
+      <c r="AK2" s="22"/>
+      <c r="AL2" s="22"/>
+      <c r="AM2" s="22"/>
+      <c r="AN2" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="AO2" s="21"/>
-      <c r="AP2" s="21"/>
-      <c r="AQ2" s="21"/>
-      <c r="AR2" s="21"/>
-      <c r="AS2" s="22"/>
-      <c r="AT2" s="20" t="s">
+      <c r="AO2" s="22"/>
+      <c r="AP2" s="22"/>
+      <c r="AQ2" s="22"/>
+      <c r="AR2" s="22"/>
+      <c r="AS2" s="23"/>
+      <c r="AT2" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="AU2" s="21"/>
-      <c r="AV2" s="21"/>
-      <c r="AW2" s="21"/>
-      <c r="AX2" s="21"/>
-      <c r="AY2" s="21"/>
-      <c r="AZ2" s="21" t="s">
+      <c r="AU2" s="22"/>
+      <c r="AV2" s="22"/>
+      <c r="AW2" s="22"/>
+      <c r="AX2" s="22"/>
+      <c r="AY2" s="22"/>
+      <c r="AZ2" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="BA2" s="21"/>
-      <c r="BB2" s="21"/>
-      <c r="BC2" s="21"/>
-      <c r="BD2" s="21"/>
+      <c r="BA2" s="22"/>
+      <c r="BB2" s="22"/>
+      <c r="BC2" s="22"/>
+      <c r="BD2" s="22"/>
       <c r="BE2" s="17"/>
     </row>
-    <row r="3" spans="1:61">
+    <row r="3" spans="1:61" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>26</v>
       </c>
@@ -8310,7 +8438,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:61">
+    <row r="4" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -8492,7 +8620,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:61">
+    <row r="5" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -8675,7 +8803,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:61">
+    <row r="6" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -8858,7 +8986,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:61">
+    <row r="7" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -9041,7 +9169,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:61">
+    <row r="8" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -9224,7 +9352,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:61">
+    <row r="9" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -9407,7 +9535,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:61">
+    <row r="10" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>60</v>
       </c>
@@ -9590,7 +9718,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:61">
+    <row r="11" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>104</v>
       </c>
@@ -9773,7 +9901,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:61">
+    <row r="12" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>105</v>
       </c>
@@ -9956,7 +10084,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:61">
+    <row r="13" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>106</v>
       </c>
@@ -10139,7 +10267,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:61">
+    <row r="14" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>107</v>
       </c>
@@ -10322,7 +10450,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:61">
+    <row r="15" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>108</v>
       </c>
@@ -10505,7 +10633,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:61">
+    <row r="16" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>109</v>
       </c>
@@ -10688,7 +10816,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:61">
+    <row r="17" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>110</v>
       </c>
@@ -10871,7 +10999,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:61">
+    <row r="18" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>111</v>
       </c>
@@ -11054,7 +11182,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:61">
+    <row r="19" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>114</v>
       </c>
@@ -11237,7 +11365,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:61">
+    <row r="20" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>115</v>
       </c>
@@ -11420,7 +11548,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:61">
+    <row r="21" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>116</v>
       </c>
@@ -11603,7 +11731,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:61">
+    <row r="22" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>117</v>
       </c>
@@ -11786,7 +11914,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:61">
+    <row r="23" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>118</v>
       </c>
@@ -11969,7 +12097,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:61">
+    <row r="24" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>119</v>
       </c>
@@ -12152,7 +12280,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:61">
+    <row r="25" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>120</v>
       </c>
@@ -12335,7 +12463,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:61">
+    <row r="26" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>121</v>
       </c>
@@ -12518,7 +12646,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:61">
+    <row r="27" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>122</v>
       </c>
@@ -12701,7 +12829,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:61">
+    <row r="28" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>123</v>
       </c>
@@ -12884,7 +13012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:61">
+    <row r="29" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>124</v>
       </c>
@@ -13067,7 +13195,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:61">
+    <row r="30" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>125</v>
       </c>
@@ -13250,7 +13378,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:61">
+    <row r="31" spans="1:61" x14ac:dyDescent="0.2">
       <c r="D31" s="11"/>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
@@ -13331,13 +13459,13 @@
   <dimension ref="A1:BI31"/>
   <sheetViews>
     <sheetView zoomScale="81" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="AT4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="BE30" sqref="C4:BE30"/>
+      <selection pane="bottomRight" activeCell="AX31" sqref="AX31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
@@ -13402,147 +13530,147 @@
     <col min="61" max="61" width="2.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61">
+    <row r="1" spans="1:61" x14ac:dyDescent="0.2">
       <c r="C1" s="6"/>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="23" t="s">
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
-      <c r="S1" s="24"/>
-      <c r="T1" s="24"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="23" t="s">
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="W1" s="24"/>
-      <c r="X1" s="24"/>
-      <c r="Y1" s="24"/>
-      <c r="Z1" s="24"/>
-      <c r="AA1" s="24"/>
-      <c r="AB1" s="24"/>
-      <c r="AC1" s="24"/>
-      <c r="AD1" s="24"/>
-      <c r="AE1" s="24"/>
-      <c r="AF1" s="24"/>
-      <c r="AG1" s="25"/>
-      <c r="AH1" s="23" t="s">
+      <c r="W1" s="18"/>
+      <c r="X1" s="18"/>
+      <c r="Y1" s="18"/>
+      <c r="Z1" s="18"/>
+      <c r="AA1" s="18"/>
+      <c r="AB1" s="18"/>
+      <c r="AC1" s="18"/>
+      <c r="AD1" s="18"/>
+      <c r="AE1" s="18"/>
+      <c r="AF1" s="18"/>
+      <c r="AG1" s="19"/>
+      <c r="AH1" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="AI1" s="24"/>
-      <c r="AJ1" s="24"/>
-      <c r="AK1" s="24"/>
-      <c r="AL1" s="24"/>
-      <c r="AM1" s="24"/>
-      <c r="AN1" s="24"/>
-      <c r="AO1" s="24"/>
-      <c r="AP1" s="24"/>
-      <c r="AQ1" s="24"/>
-      <c r="AR1" s="24"/>
-      <c r="AS1" s="25"/>
-      <c r="AT1" s="23" t="s">
+      <c r="AI1" s="18"/>
+      <c r="AJ1" s="18"/>
+      <c r="AK1" s="18"/>
+      <c r="AL1" s="18"/>
+      <c r="AM1" s="18"/>
+      <c r="AN1" s="18"/>
+      <c r="AO1" s="18"/>
+      <c r="AP1" s="18"/>
+      <c r="AQ1" s="18"/>
+      <c r="AR1" s="18"/>
+      <c r="AS1" s="19"/>
+      <c r="AT1" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="AU1" s="24"/>
-      <c r="AV1" s="24"/>
-      <c r="AW1" s="24"/>
-      <c r="AX1" s="24"/>
-      <c r="AY1" s="24"/>
-      <c r="AZ1" s="24"/>
-      <c r="BA1" s="24"/>
-      <c r="BB1" s="24"/>
-      <c r="BC1" s="24"/>
-      <c r="BD1" s="24"/>
-      <c r="BE1" s="25"/>
+      <c r="AU1" s="18"/>
+      <c r="AV1" s="18"/>
+      <c r="AW1" s="18"/>
+      <c r="AX1" s="18"/>
+      <c r="AY1" s="18"/>
+      <c r="AZ1" s="18"/>
+      <c r="BA1" s="18"/>
+      <c r="BB1" s="18"/>
+      <c r="BC1" s="18"/>
+      <c r="BD1" s="18"/>
+      <c r="BE1" s="19"/>
     </row>
-    <row r="2" spans="1:61">
+    <row r="2" spans="1:61" x14ac:dyDescent="0.2">
       <c r="C2" s="1"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="20" t="s">
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21" t="s">
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="21"/>
-      <c r="T2" s="21"/>
-      <c r="U2" s="22"/>
-      <c r="V2" s="20" t="s">
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="22"/>
+      <c r="U2" s="23"/>
+      <c r="V2" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="W2" s="21"/>
-      <c r="X2" s="21"/>
-      <c r="Y2" s="21"/>
-      <c r="Z2" s="21"/>
-      <c r="AA2" s="21"/>
-      <c r="AB2" s="21" t="s">
+      <c r="W2" s="22"/>
+      <c r="X2" s="22"/>
+      <c r="Y2" s="22"/>
+      <c r="Z2" s="22"/>
+      <c r="AA2" s="22"/>
+      <c r="AB2" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="AC2" s="21"/>
-      <c r="AD2" s="21"/>
-      <c r="AE2" s="21"/>
-      <c r="AF2" s="21"/>
+      <c r="AC2" s="22"/>
+      <c r="AD2" s="22"/>
+      <c r="AE2" s="22"/>
+      <c r="AF2" s="22"/>
       <c r="AG2" s="17"/>
-      <c r="AH2" s="20" t="s">
+      <c r="AH2" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="AI2" s="21"/>
-      <c r="AJ2" s="21"/>
-      <c r="AK2" s="21"/>
-      <c r="AL2" s="21"/>
-      <c r="AM2" s="21"/>
-      <c r="AN2" s="21" t="s">
+      <c r="AI2" s="22"/>
+      <c r="AJ2" s="22"/>
+      <c r="AK2" s="22"/>
+      <c r="AL2" s="22"/>
+      <c r="AM2" s="22"/>
+      <c r="AN2" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="AO2" s="21"/>
-      <c r="AP2" s="21"/>
-      <c r="AQ2" s="21"/>
-      <c r="AR2" s="21"/>
-      <c r="AS2" s="22"/>
-      <c r="AT2" s="20" t="s">
+      <c r="AO2" s="22"/>
+      <c r="AP2" s="22"/>
+      <c r="AQ2" s="22"/>
+      <c r="AR2" s="22"/>
+      <c r="AS2" s="23"/>
+      <c r="AT2" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="AU2" s="21"/>
-      <c r="AV2" s="21"/>
-      <c r="AW2" s="21"/>
-      <c r="AX2" s="21"/>
-      <c r="AY2" s="21"/>
-      <c r="AZ2" s="21" t="s">
+      <c r="AU2" s="22"/>
+      <c r="AV2" s="22"/>
+      <c r="AW2" s="22"/>
+      <c r="AX2" s="22"/>
+      <c r="AY2" s="22"/>
+      <c r="AZ2" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="BA2" s="21"/>
-      <c r="BB2" s="21"/>
-      <c r="BC2" s="21"/>
-      <c r="BD2" s="21"/>
+      <c r="BA2" s="22"/>
+      <c r="BB2" s="22"/>
+      <c r="BC2" s="22"/>
+      <c r="BD2" s="22"/>
       <c r="BE2" s="17"/>
     </row>
-    <row r="3" spans="1:61">
+    <row r="3" spans="1:61" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>26</v>
       </c>
@@ -13659,7 +13787,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:61">
+    <row r="4" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -13841,7 +13969,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:61">
+    <row r="5" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -14024,7 +14152,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:61">
+    <row r="6" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -14207,7 +14335,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:61">
+    <row r="7" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -14390,7 +14518,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:61">
+    <row r="8" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -14573,7 +14701,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:61">
+    <row r="9" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -14756,7 +14884,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:61">
+    <row r="10" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>60</v>
       </c>
@@ -14939,7 +15067,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:61">
+    <row r="11" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>104</v>
       </c>
@@ -15122,7 +15250,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:61">
+    <row r="12" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>105</v>
       </c>
@@ -15305,7 +15433,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:61">
+    <row r="13" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>106</v>
       </c>
@@ -15488,7 +15616,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:61">
+    <row r="14" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>107</v>
       </c>
@@ -15671,7 +15799,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:61">
+    <row r="15" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>108</v>
       </c>
@@ -15854,7 +15982,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:61">
+    <row r="16" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>109</v>
       </c>
@@ -16037,7 +16165,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:61">
+    <row r="17" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>110</v>
       </c>
@@ -16220,7 +16348,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:61">
+    <row r="18" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>111</v>
       </c>
@@ -16403,7 +16531,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:61">
+    <row r="19" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>114</v>
       </c>
@@ -16586,7 +16714,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:61">
+    <row r="20" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>115</v>
       </c>
@@ -16769,7 +16897,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:61">
+    <row r="21" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>116</v>
       </c>
@@ -16952,7 +17080,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:61">
+    <row r="22" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>117</v>
       </c>
@@ -17135,7 +17263,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:61">
+    <row r="23" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>118</v>
       </c>
@@ -17318,7 +17446,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:61">
+    <row r="24" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>119</v>
       </c>
@@ -17501,7 +17629,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:61">
+    <row r="25" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>120</v>
       </c>
@@ -17684,7 +17812,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:61">
+    <row r="26" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>121</v>
       </c>
@@ -17867,7 +17995,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:61">
+    <row r="27" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>122</v>
       </c>
@@ -18050,7 +18178,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:61">
+    <row r="28" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>123</v>
       </c>
@@ -18233,7 +18361,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:61">
+    <row r="29" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>124</v>
       </c>
@@ -18416,7 +18544,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:61">
+    <row r="30" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>125</v>
       </c>
@@ -18599,7 +18727,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:61">
+    <row r="31" spans="1:61" x14ac:dyDescent="0.2">
       <c r="D31" s="11"/>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
@@ -18677,16 +18805,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F38DBB4D-9BB4-FC4D-AB7A-FD8E16FA5798}">
-  <dimension ref="A1:AK15"/>
+  <dimension ref="A1:AC15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="R4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomRight" activeCell="Y15" sqref="Y15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
@@ -18696,122 +18824,106 @@
     <col min="6" max="6" width="2.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="1.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="1.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="1.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="1.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="1.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="1.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="1.33203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="1.33203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="1.33203125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="1.6640625" customWidth="1"/>
-    <col min="35" max="35" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="255.6640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="1.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="1.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="1.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="1.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="1.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="1.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="1.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="1.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="1.6640625" customWidth="1"/>
+    <col min="27" max="27" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="255.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="2.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="C1" s="6"/>
-      <c r="D1" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="24" t="s">
-        <v>182</v>
-      </c>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
-      <c r="S1" s="24"/>
-      <c r="T1" s="24"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="24"/>
-      <c r="X1" s="24"/>
-      <c r="Y1" s="24"/>
-      <c r="Z1" s="24"/>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC1" s="24"/>
-      <c r="AD1" s="24"/>
-      <c r="AE1" s="24"/>
-      <c r="AF1" s="24"/>
-      <c r="AG1" s="25"/>
+      <c r="D1" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="18" t="s">
+        <v>233</v>
+      </c>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="18" t="s">
+        <v>238</v>
+      </c>
+      <c r="W1" s="18"/>
+      <c r="X1" s="18"/>
+      <c r="Y1" s="19"/>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="C2" s="1"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="N2" s="21"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22" t="s">
+        <v>235</v>
+      </c>
+      <c r="M2" s="23"/>
+      <c r="N2" s="22" t="s">
+        <v>234</v>
+      </c>
       <c r="O2" s="22"/>
-      <c r="P2" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="T2" s="21"/>
-      <c r="U2" s="22"/>
-      <c r="V2" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="W2" s="21"/>
-      <c r="X2" s="21"/>
-      <c r="Y2" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="Z2" s="21"/>
-      <c r="AA2" s="22"/>
-      <c r="AB2" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="AC2" s="21"/>
-      <c r="AD2" s="21"/>
-      <c r="AE2" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="AF2" s="21"/>
-      <c r="AG2" s="22"/>
+      <c r="P2" s="22" t="s">
+        <v>235</v>
+      </c>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="S2" s="22"/>
+      <c r="T2" s="22" t="s">
+        <v>235</v>
+      </c>
+      <c r="U2" s="23"/>
+      <c r="V2" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="W2" s="22"/>
+      <c r="X2" s="22" t="s">
+        <v>235</v>
+      </c>
+      <c r="Y2" s="23"/>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>26</v>
       </c>
@@ -18828,51 +18940,43 @@
         <v>33</v>
       </c>
       <c r="I3" s="9"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8" t="s">
+      <c r="J3" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="9"/>
       <c r="N3" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="O3" s="9"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="R3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="S3" s="8"/>
       <c r="T3" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="U3" s="9"/>
+      <c r="V3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="U3" s="9"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA3" s="9"/>
-      <c r="AB3" s="8"/>
-      <c r="AC3" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD3" s="8"/>
-      <c r="AE3" s="8"/>
-      <c r="AF3" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="AG3" s="9"/>
-      <c r="AI3" t="s">
+      <c r="Y3" s="9"/>
+      <c r="AA3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:37">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -18883,106 +18987,82 @@
         <v>13</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" s="13" t="s">
+      <c r="I4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K4" s="18" t="s">
+      <c r="K4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M4" s="2" t="s">
+      <c r="M4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="N4" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T4" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="O4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q4" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="T4" s="19" t="s">
+      <c r="U4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="X4" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="U4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="W4" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="X4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z4" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="AA4" s="3" t="s">
-        <v>2</v>
+      <c r="Y4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>13</v>
       </c>
       <c r="AB4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC4" s="13" t="s">
-        <v>188</v>
-      </c>
-      <c r="AD4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF4" s="19" t="s">
         <v>192</v>
       </c>
-      <c r="AG4" s="3" t="s">
+      <c r="AC4" t="s">
         <v>15</v>
       </c>
-      <c r="AI4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>193</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="5" spans="1:37">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -19000,100 +19080,76 @@
         <v>2</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="2">
-        <v>0</v>
+      <c r="H5" s="2" t="s">
+        <v>193</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K5" s="2">
-        <v>0</v>
+        <v>194</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N5" s="2">
-        <v>0</v>
-      </c>
-      <c r="O5" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="O5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q5" s="2">
-        <v>0</v>
+        <v>197</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>2</v>
+        <v>198</v>
       </c>
       <c r="S5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="T5" s="2">
-        <v>0</v>
+      <c r="T5" s="2" t="s">
+        <v>199</v>
       </c>
       <c r="U5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="W5" s="2">
-        <v>0</v>
+        <v>200</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="X5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z5" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="3" t="s">
-        <v>2</v>
+        <v>201</v>
+      </c>
+      <c r="Y5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>14</v>
       </c>
       <c r="AB5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC5" s="2">
-        <v>0</v>
-      </c>
-      <c r="AD5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF5" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG5" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="AC5" t="s">
         <v>15</v>
       </c>
-      <c r="AI5" t="s">
-        <v>14</v>
-      </c>
-      <c r="AJ5" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="6" spans="1:37">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -19104,107 +19160,83 @@
       <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="2">
-        <v>0</v>
+      <c r="D6" s="2" t="s">
+        <v>183</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="2">
-        <v>0</v>
+      <c r="F6" s="2" t="s">
+        <v>193</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>32</v>
+        <v>203</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K6" s="2">
-        <v>0</v>
+        <v>204</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N6" s="2">
-        <v>0</v>
-      </c>
-      <c r="O6" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="O6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q6" s="2">
-        <v>0</v>
+        <v>207</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>2</v>
+        <v>208</v>
       </c>
       <c r="S6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="T6" s="2">
-        <v>0</v>
+      <c r="T6" s="2" t="s">
+        <v>209</v>
       </c>
       <c r="U6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="W6" s="2">
-        <v>0</v>
+        <v>210</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="X6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="3" t="s">
-        <v>2</v>
+        <v>211</v>
+      </c>
+      <c r="Y6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>14</v>
       </c>
       <c r="AB6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AD6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG6" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="AC6" t="s">
         <v>15</v>
       </c>
-      <c r="AI6" t="s">
-        <v>14</v>
-      </c>
-      <c r="AJ6" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="AK6" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -19215,107 +19247,83 @@
       <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="2">
-        <v>0</v>
+      <c r="D7" s="2" t="s">
+        <v>184</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="2">
-        <v>0</v>
+      <c r="F7" s="2" t="s">
+        <v>194</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H7" s="2">
-        <v>0</v>
+      <c r="H7" s="2" t="s">
+        <v>204</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J7" s="14" t="s">
-        <v>2</v>
+      <c r="J7" s="2" t="s">
+        <v>213</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="L7" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="M7" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="N7" s="14">
-        <v>0</v>
-      </c>
-      <c r="O7" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="P7" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q7" s="14">
-        <v>0</v>
-      </c>
-      <c r="R7" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="S7" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="T7" s="14">
+        <v>2</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="M7" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="N7" s="2">
+        <v>0</v>
+      </c>
+      <c r="O7" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="P7" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R7" s="2">
+        <v>0</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T7" s="2">
         <v>0</v>
       </c>
       <c r="U7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="V7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="W7" s="2">
-        <v>0</v>
-      </c>
-      <c r="X7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="3" t="s">
-        <v>2</v>
+      <c r="V7" s="2">
+        <v>0</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="X7" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>14</v>
       </c>
       <c r="AB7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AD7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG7" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="AC7" t="s">
         <v>15</v>
       </c>
-      <c r="AI7" t="s">
-        <v>14</v>
-      </c>
-      <c r="AJ7" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="AK7" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="8" spans="1:37">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -19326,107 +19334,83 @@
       <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="2">
-        <v>0</v>
+      <c r="D8" s="2" t="s">
+        <v>185</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="2">
-        <v>0</v>
+      <c r="F8" s="2" t="s">
+        <v>195</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H8" s="2">
-        <v>0</v>
+      <c r="H8" s="2" t="s">
+        <v>205</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J8" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="K8" s="14">
-        <v>0</v>
-      </c>
-      <c r="L8" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="M8" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="N8" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="O8" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="P8" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q8" s="14">
-        <v>0</v>
-      </c>
-      <c r="R8" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="S8" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="T8" s="14">
+      <c r="J8" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="K8" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="M8" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="N8" s="2">
+        <v>0</v>
+      </c>
+      <c r="O8" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="P8" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R8" s="2">
+        <v>0</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T8" s="2">
         <v>0</v>
       </c>
       <c r="U8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="V8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="W8" s="2">
-        <v>0</v>
-      </c>
-      <c r="X8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z8" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA8" s="3" t="s">
-        <v>2</v>
+      <c r="V8" s="2">
+        <v>0</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="X8" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>14</v>
       </c>
       <c r="AB8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC8" s="2">
-        <v>0</v>
-      </c>
-      <c r="AD8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF8" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG8" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="AC8" t="s">
         <v>15</v>
       </c>
-      <c r="AI8" t="s">
-        <v>14</v>
-      </c>
-      <c r="AJ8" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="AK8" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="9" spans="1:37">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -19437,107 +19421,83 @@
       <c r="C9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="2">
-        <v>0</v>
+      <c r="D9" s="2" t="s">
+        <v>186</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="2">
-        <v>0</v>
+      <c r="F9" s="2" t="s">
+        <v>196</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H9" s="2">
-        <v>0</v>
+      <c r="H9" s="2" t="s">
+        <v>206</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J9" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="K9" s="14">
-        <v>0</v>
-      </c>
-      <c r="L9" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="M9" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="N9" s="14">
-        <v>0</v>
-      </c>
-      <c r="O9" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="P9" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q9" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="R9" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="S9" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="T9" s="14">
+      <c r="J9" s="2">
+        <v>0</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0</v>
+      </c>
+      <c r="M9" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="O9" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R9" s="2">
+        <v>0</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T9" s="2">
         <v>0</v>
       </c>
       <c r="U9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="V9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="W9" s="2">
-        <v>0</v>
-      </c>
-      <c r="X9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA9" s="3" t="s">
-        <v>2</v>
+      <c r="V9" s="2">
+        <v>0</v>
+      </c>
+      <c r="W9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="X9" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>14</v>
       </c>
       <c r="AB9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AD9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG9" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="AC9" t="s">
         <v>15</v>
       </c>
-      <c r="AI9" t="s">
-        <v>14</v>
-      </c>
-      <c r="AJ9" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="AK9" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="10" spans="1:37">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>60</v>
       </c>
@@ -19548,107 +19508,83 @@
       <c r="C10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="2">
-        <v>0</v>
+      <c r="D10" s="2" t="s">
+        <v>187</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="2">
-        <v>0</v>
+      <c r="F10" s="2" t="s">
+        <v>197</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H10" s="2">
-        <v>0</v>
+      <c r="H10" s="2" t="s">
+        <v>207</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J10" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="K10" s="14">
-        <v>0</v>
-      </c>
-      <c r="L10" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="M10" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="N10" s="14">
-        <v>0</v>
-      </c>
-      <c r="O10" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="P10" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q10" s="14">
-        <v>0</v>
-      </c>
-      <c r="R10" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="S10" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="T10" s="14" t="s">
-        <v>66</v>
+      <c r="J10" s="2">
+        <v>0</v>
+      </c>
+      <c r="K10" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0</v>
+      </c>
+      <c r="M10" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="O10" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R10" s="2">
+        <v>0</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T10" s="2">
+        <v>0</v>
       </c>
       <c r="U10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="V10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="W10" s="2">
-        <v>0</v>
-      </c>
-      <c r="X10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA10" s="3" t="s">
-        <v>2</v>
+      <c r="V10" s="2">
+        <v>0</v>
+      </c>
+      <c r="W10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="X10" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>14</v>
       </c>
       <c r="AB10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AD10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG10" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="AC10" t="s">
         <v>15</v>
       </c>
-      <c r="AI10" t="s">
-        <v>14</v>
-      </c>
-      <c r="AJ10" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="AK10" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="11" spans="1:37">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>114</v>
       </c>
@@ -19659,107 +19595,83 @@
       <c r="C11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="2">
-        <v>0</v>
+      <c r="D11" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="2">
-        <v>0</v>
+      <c r="F11" s="2" t="s">
+        <v>198</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H11" s="2">
-        <v>0</v>
+      <c r="H11" s="2" t="s">
+        <v>208</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K11" s="2">
-        <v>0</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M11" s="2" t="s">
+      <c r="J11" s="2">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0</v>
+      </c>
+      <c r="M11" s="3" t="s">
         <v>2</v>
       </c>
       <c r="N11" s="2">
         <v>0</v>
       </c>
-      <c r="O11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="P11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q11" s="2">
-        <v>0</v>
+      <c r="O11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P11" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="S11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="T11" s="2">
-        <v>0</v>
-      </c>
-      <c r="U11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="V11" s="14" t="s">
-        <v>2</v>
+        <v>223</v>
+      </c>
+      <c r="S11" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="U11" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="V11" s="2">
+        <v>0</v>
       </c>
       <c r="W11" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="X11" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y11" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z11" s="14">
-        <v>0</v>
-      </c>
-      <c r="AA11" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB11" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC11" s="14">
-        <v>0</v>
-      </c>
-      <c r="AD11" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE11" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF11" s="14">
-        <v>0</v>
-      </c>
-      <c r="AG11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="X11" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AI11" t="s">
+      <c r="AA11" t="s">
         <v>14</v>
       </c>
-      <c r="AJ11" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="AK11" t="s">
+      <c r="AB11" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="AC11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>115</v>
       </c>
@@ -19770,107 +19682,83 @@
       <c r="C12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="2">
-        <v>0</v>
+      <c r="D12" s="2" t="s">
+        <v>189</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="2">
-        <v>0</v>
+      <c r="F12" s="2" t="s">
+        <v>199</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H12" s="2">
-        <v>0</v>
+      <c r="H12" s="2" t="s">
+        <v>209</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K12" s="2">
-        <v>0</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M12" s="2" t="s">
+      <c r="J12" s="2">
+        <v>0</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0</v>
+      </c>
+      <c r="M12" s="3" t="s">
         <v>2</v>
       </c>
       <c r="N12" s="2">
         <v>0</v>
       </c>
-      <c r="O12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="P12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q12" s="2">
-        <v>0</v>
+      <c r="O12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P12" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="S12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="T12" s="2">
-        <v>0</v>
-      </c>
-      <c r="U12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="V12" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="W12" s="14">
-        <v>0</v>
-      </c>
-      <c r="X12" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y12" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z12" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA12" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB12" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC12" s="14">
-        <v>0</v>
-      </c>
-      <c r="AD12" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE12" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF12" s="14">
-        <v>0</v>
-      </c>
-      <c r="AG12" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="S12" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="U12" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="V12" s="2">
+        <v>0</v>
+      </c>
+      <c r="W12" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="X12" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AI12" t="s">
+      <c r="AA12" t="s">
         <v>14</v>
       </c>
-      <c r="AJ12" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="AK12" t="s">
+      <c r="AB12" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="AC12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:37">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>116</v>
       </c>
@@ -19881,107 +19769,83 @@
       <c r="C13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="2">
-        <v>0</v>
+      <c r="D13" s="2" t="s">
+        <v>190</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="2">
-        <v>0</v>
+      <c r="F13" s="2" t="s">
+        <v>200</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H13" s="2">
-        <v>0</v>
+      <c r="H13" s="2" t="s">
+        <v>210</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K13" s="2">
-        <v>0</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M13" s="2" t="s">
+      <c r="J13" s="2">
+        <v>0</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0</v>
+      </c>
+      <c r="M13" s="3" t="s">
         <v>2</v>
       </c>
       <c r="N13" s="2">
         <v>0</v>
       </c>
-      <c r="O13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="P13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q13" s="2">
-        <v>0</v>
-      </c>
-      <c r="R13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="S13" s="2" t="s">
+      <c r="O13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P13" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R13" s="2">
+        <v>0</v>
+      </c>
+      <c r="S13" s="14" t="s">
         <v>2</v>
       </c>
       <c r="T13" s="2">
         <v>0</v>
       </c>
-      <c r="U13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="V13" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="W13" s="14">
-        <v>0</v>
-      </c>
-      <c r="X13" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y13" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z13" s="14">
-        <v>0</v>
-      </c>
-      <c r="AA13" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB13" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC13" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="AD13" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE13" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF13" s="14">
-        <v>0</v>
-      </c>
-      <c r="AG13" s="3" t="s">
+      <c r="U13" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="V13" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="W13" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="X13" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="Y13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AI13" t="s">
+      <c r="AA13" t="s">
         <v>14</v>
       </c>
-      <c r="AJ13" s="12" t="s">
-        <v>180</v>
-      </c>
-      <c r="AK13" t="s">
+      <c r="AB13" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="AC13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:37">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>117</v>
       </c>
@@ -19992,107 +19856,83 @@
       <c r="C14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="2">
-        <v>0</v>
+      <c r="D14" s="2" t="s">
+        <v>191</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F14" s="2">
-        <v>0</v>
+      <c r="F14" s="2" t="s">
+        <v>201</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H14" s="2">
-        <v>0</v>
+      <c r="H14" s="2" t="s">
+        <v>211</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K14" s="2">
-        <v>0</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M14" s="2" t="s">
+      <c r="J14" s="2">
+        <v>0</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L14" s="2">
+        <v>0</v>
+      </c>
+      <c r="M14" s="3" t="s">
         <v>2</v>
       </c>
       <c r="N14" s="2">
         <v>0</v>
       </c>
-      <c r="O14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="P14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q14" s="2">
-        <v>0</v>
-      </c>
-      <c r="R14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="S14" s="2" t="s">
+      <c r="O14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P14" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R14" s="2">
+        <v>0</v>
+      </c>
+      <c r="S14" s="14" t="s">
         <v>2</v>
       </c>
       <c r="T14" s="2">
         <v>0</v>
       </c>
-      <c r="U14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="V14" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="W14" s="14">
-        <v>0</v>
-      </c>
-      <c r="X14" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y14" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z14" s="14">
-        <v>0</v>
-      </c>
-      <c r="AA14" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB14" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC14" s="14">
-        <v>0</v>
-      </c>
-      <c r="AD14" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE14" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF14" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="AG14" s="3" t="s">
+      <c r="U14" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="V14" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="W14" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="X14" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="Y14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB14" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="AC14" t="s">
         <v>15</v>
       </c>
-      <c r="AI14" t="s">
-        <v>14</v>
-      </c>
-      <c r="AJ14" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="AK14" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="15" spans="1:37">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
@@ -20114,31 +19954,23 @@
       <c r="V15" s="11"/>
       <c r="W15" s="11"/>
       <c r="X15" s="11"/>
-      <c r="Y15" s="11"/>
-      <c r="Z15" s="11"/>
-      <c r="AA15" s="11"/>
-      <c r="AB15" s="11"/>
-      <c r="AC15" s="11"/>
-      <c r="AD15" s="11"/>
-      <c r="AE15" s="11"/>
-      <c r="AF15" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
     <mergeCell ref="D2:I2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:O2"/>
     <mergeCell ref="D1:I1"/>
-    <mergeCell ref="J1:O1"/>
-    <mergeCell ref="P1:U1"/>
-    <mergeCell ref="V1:AA1"/>
-    <mergeCell ref="AB1:AG1"/>
-    <mergeCell ref="V2:X2"/>
-    <mergeCell ref="Y2:AA2"/>
-    <mergeCell ref="AB2:AD2"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="AE2:AG2"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="P2:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20150,7 +19982,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>